<commit_message>
Mejoras al plan de proyecto
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Horas insumidas" sheetId="2" r:id="rId2"/>
     <sheet name="Estadísticas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="114210"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="75">
   <si>
     <t>Id</t>
   </si>
@@ -231,10 +231,16 @@
     <t>Reporte de avance</t>
   </si>
   <si>
-    <t>munita de reunion</t>
-  </si>
-  <si>
     <t>Indicador FC</t>
+  </si>
+  <si>
+    <t>Minuta de reunion</t>
+  </si>
+  <si>
+    <t>Total Sprint</t>
+  </si>
+  <si>
+    <t>Creación de subtasks de stories</t>
   </si>
 </sst>
 </file>
@@ -307,7 +313,9 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -317,8 +325,12 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -328,7 +340,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -350,6 +364,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -359,7 +374,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -374,7 +388,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="es-AR"/>
   <c:chart>
     <c:plotArea>
       <c:layout>
@@ -382,10 +396,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="6.8750000000000006E-2"/>
+          <c:x val="6.8750000000000019E-2"/>
           <c:y val="4.8611111111111112E-2"/>
-          <c:w val="0.70416666666666672"/>
-          <c:h val="0.82986111111111116"/>
+          <c:w val="0.7041666666666665"/>
+          <c:h val="0.82986111111111138"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -433,11 +447,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="39604992"/>
-        <c:axId val="39606912"/>
+        <c:axId val="72078080"/>
+        <c:axId val="72079616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="39604992"/>
+        <c:axId val="72078080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -458,15 +472,15 @@
                 <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39606912"/>
+        <c:crossAx val="72079616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="39606912"/>
+        <c:axId val="72079616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -474,7 +488,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39604992"/>
+        <c:crossAx val="72078080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -487,7 +501,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -531,7 +545,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -890,7 +904,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$124,A2,'Horas insumidas'!$F$6:$F$124)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$125,A2,'Horas insumidas'!$F$6:$F$125)*$B$15</f>
         <v>0</v>
       </c>
       <c r="H2">
@@ -931,12 +945,12 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$124,A3,'Horas insumidas'!$F$6:$F$124)*$B$15</f>
-        <v>51.5</v>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$125,A3,'Horas insumidas'!$F$6:$F$125)*$B$15</f>
+        <v>22</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H11" si="0">F3-G3</f>
-        <v>-51.5</v>
+        <v>-22</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I11" si="1">F3-E3</f>
@@ -972,7 +986,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$124,A4,'Horas insumidas'!$F$6:$F$124)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$125,A4,'Horas insumidas'!$F$6:$F$125)*$B$15</f>
         <v>0</v>
       </c>
       <c r="H4">
@@ -1013,7 +1027,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$124,A5,'Horas insumidas'!$F$6:$F$124)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$125,A5,'Horas insumidas'!$F$6:$F$125)*$B$15</f>
         <v>0</v>
       </c>
       <c r="H5">
@@ -1054,7 +1068,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$124,A6,'Horas insumidas'!$F$6:$F$124)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$125,A6,'Horas insumidas'!$F$6:$F$125)*$B$15</f>
         <v>0</v>
       </c>
       <c r="H6">
@@ -1095,7 +1109,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$124,A7,'Horas insumidas'!$F$6:$F$124)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$125,A7,'Horas insumidas'!$F$6:$F$125)*$B$15</f>
         <v>0</v>
       </c>
       <c r="H7">
@@ -1136,7 +1150,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$124,A8,'Horas insumidas'!$F$6:$F$124)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$125,A8,'Horas insumidas'!$F$6:$F$125)*$B$15</f>
         <v>0</v>
       </c>
       <c r="H8">
@@ -1177,7 +1191,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$124,A9,'Horas insumidas'!$F$6:$F$124)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$125,A9,'Horas insumidas'!$F$6:$F$125)*$B$15</f>
         <v>0</v>
       </c>
       <c r="H9">
@@ -1218,7 +1232,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$124,A10,'Horas insumidas'!$F$6:$F$124)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$125,A10,'Horas insumidas'!$F$6:$F$125)*$B$15</f>
         <v>0</v>
       </c>
       <c r="H10">
@@ -1259,7 +1273,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$124,A11,'Horas insumidas'!$F$6:$F$124)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$125,A11,'Horas insumidas'!$F$6:$F$125)*$B$15</f>
         <v>0</v>
       </c>
       <c r="H11">
@@ -1293,11 +1307,11 @@
       </c>
       <c r="G12">
         <f>SUM(G2:G11)</f>
-        <v>51.5</v>
+        <v>22</v>
       </c>
       <c r="H12">
         <f>SUM(H2:H11)</f>
-        <v>-51.5</v>
+        <v>-22</v>
       </c>
       <c r="I12">
         <f>SUM(I2:I11)</f>
@@ -1322,7 +1336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
@@ -1337,19 +1351,19 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1363,9 +1377,6 @@
       <c r="D3" t="s">
         <v>54</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
       <c r="F3">
         <v>2</v>
       </c>
@@ -1394,9 +1405,6 @@
       <c r="D5" t="s">
         <v>55</v>
       </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
       <c r="F5">
         <v>1.5</v>
       </c>
@@ -1411,9 +1419,6 @@
       <c r="D6" t="s">
         <v>56</v>
       </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
       <c r="F6">
         <v>3</v>
       </c>
@@ -1428,9 +1433,6 @@
       <c r="D7" t="s">
         <v>52</v>
       </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
       <c r="F7">
         <v>4</v>
       </c>
@@ -1445,9 +1447,6 @@
       <c r="D8" t="s">
         <v>57</v>
       </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
       <c r="F8">
         <v>0.5</v>
       </c>
@@ -1462,9 +1461,6 @@
       <c r="D9" t="s">
         <v>54</v>
       </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
       <c r="F9">
         <v>2</v>
       </c>
@@ -1479,9 +1475,6 @@
       <c r="D10" t="s">
         <v>55</v>
       </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
       <c r="F10">
         <v>2</v>
       </c>
@@ -1495,9 +1488,6 @@
       </c>
       <c r="D11" t="s">
         <v>52</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
       </c>
       <c r="F11">
         <v>6</v>
@@ -1539,9 +1529,6 @@
       <c r="D14" t="s">
         <v>58</v>
       </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
       <c r="F14">
         <v>4</v>
       </c>
@@ -1556,9 +1543,6 @@
       <c r="D15" t="s">
         <v>59</v>
       </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
       <c r="F15">
         <v>1.5</v>
       </c>
@@ -1573,9 +1557,6 @@
       <c r="D16" t="s">
         <v>54</v>
       </c>
-      <c r="E16" t="s">
-        <v>11</v>
-      </c>
       <c r="F16">
         <v>1</v>
       </c>
@@ -1590,9 +1571,6 @@
       <c r="D17" t="s">
         <v>55</v>
       </c>
-      <c r="E17" t="s">
-        <v>11</v>
-      </c>
       <c r="F17">
         <v>1</v>
       </c>
@@ -1720,9 +1698,6 @@
       <c r="D25" t="s">
         <v>58</v>
       </c>
-      <c r="E25" t="s">
-        <v>11</v>
-      </c>
       <c r="F25">
         <v>1</v>
       </c>
@@ -1737,9 +1712,6 @@
       <c r="D26" t="s">
         <v>59</v>
       </c>
-      <c r="E26" t="s">
-        <v>11</v>
-      </c>
       <c r="F26">
         <v>1</v>
       </c>
@@ -1786,10 +1758,7 @@
         <v>53</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
-      </c>
-      <c r="E29" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1803,10 +1772,7 @@
         <v>53</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
-      </c>
-      <c r="E30" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1822,30 +1788,52 @@
       <c r="D31" t="s">
         <v>70</v>
       </c>
-      <c r="E31" t="s">
-        <v>11</v>
-      </c>
       <c r="F31">
         <v>0.5</v>
       </c>
     </row>
     <row r="32" spans="2:6">
-      <c r="B32" s="1"/>
+      <c r="B32" s="1">
+        <v>40444</v>
+      </c>
+      <c r="C32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" t="s">
+        <v>58</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="2:6">
-      <c r="B33" s="1"/>
+      <c r="B33" s="1">
+        <v>40444</v>
+      </c>
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="2:6">
-      <c r="B34" s="1"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" s="3">
+        <f>SUM(F3:F33)</f>
+        <v>61.5</v>
+      </c>
     </row>
     <row r="35" spans="2:6">
-      <c r="E35" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F35" s="6">
-        <f>SUM(F3:F27)</f>
-        <v>55</v>
-      </c>
+      <c r="B35" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Se agrega la funcionalidad completa real de desarrollo. Se agregan horas trabajadas.
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Earned Value" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="77">
   <si>
     <t>Id</t>
   </si>
@@ -27,9 +27,6 @@
     <t>Estado</t>
   </si>
   <si>
-    <t>% Avance esperado (50-50)</t>
-  </si>
-  <si>
     <t>PV</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>Crear, Modificar y Eliminar campañas</t>
   </si>
   <si>
-    <t>En Curso</t>
-  </si>
-  <si>
     <t>S-01003</t>
   </si>
   <si>
@@ -247,6 +241,12 @@
   </si>
   <si>
     <t>Actualizacion de datos Version One</t>
+  </si>
+  <si>
+    <t>Completada</t>
+  </si>
+  <si>
+    <t>% Avance esperado (0-50-100)</t>
   </si>
 </sst>
 </file>
@@ -458,11 +458,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="65590784"/>
-        <c:axId val="65592320"/>
+        <c:axId val="88480000"/>
+        <c:axId val="88485888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65590784"/>
+        <c:axId val="88480000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -486,12 +486,12 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65592320"/>
+        <c:crossAx val="88485888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65592320"/>
+        <c:axId val="88485888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -499,20 +499,21 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65590784"/>
+        <c:crossAx val="88480000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -842,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -851,7 +852,7 @@
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="51.85546875" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.140625" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" customWidth="1"/>
@@ -870,39 +871,39 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -915,12 +916,12 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$128,A2,'Horas insumidas'!$F$6:$F$128)*$B$15</f>
-        <v>27</v>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A2,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
+        <v>30</v>
       </c>
       <c r="H2">
         <f>F2-G2</f>
-        <v>-27</v>
+        <v>-30</v>
       </c>
       <c r="I2">
         <f>F2-E2</f>
@@ -937,16 +938,16 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="D3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E3">
         <f>40*B15</f>
@@ -956,7 +957,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$128,A3,'Horas insumidas'!$F$6:$F$128)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A3,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
         <v>0</v>
       </c>
       <c r="H3">
@@ -978,13 +979,13 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -997,12 +998,12 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$128,A4,'Horas insumidas'!$F$6:$F$128)*$B$15</f>
-        <v>0</v>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A4,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
+        <v>3</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
@@ -1012,20 +1013,20 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K4" t="e">
+      <c r="K4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1038,7 +1039,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$128,A5,'Horas insumidas'!$F$6:$F$128)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A5,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
         <v>0</v>
       </c>
       <c r="H5">
@@ -1060,13 +1061,13 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1079,7 +1080,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$128,A6,'Horas insumidas'!$F$6:$F$128)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A6,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
         <v>0</v>
       </c>
       <c r="H6">
@@ -1101,13 +1102,13 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1120,7 +1121,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$128,A7,'Horas insumidas'!$F$6:$F$128)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A7,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
         <v>0</v>
       </c>
       <c r="H7">
@@ -1142,13 +1143,13 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1161,7 +1162,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$128,A8,'Horas insumidas'!$F$6:$F$128)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A8,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
         <v>0</v>
       </c>
       <c r="H8">
@@ -1183,13 +1184,13 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1202,7 +1203,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$128,A9,'Horas insumidas'!$F$6:$F$128)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A9,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
         <v>0</v>
       </c>
       <c r="H9">
@@ -1224,13 +1225,13 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1243,7 +1244,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$128,A10,'Horas insumidas'!$F$6:$F$128)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A10,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
         <v>0</v>
       </c>
       <c r="H10">
@@ -1265,13 +1266,13 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1284,7 +1285,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$128,A11,'Horas insumidas'!$F$6:$F$128)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A11,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
         <v>0</v>
       </c>
       <c r="H11">
@@ -1306,7 +1307,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="D12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12">
         <f>SUM(E2:E11)</f>
@@ -1318,11 +1319,11 @@
       </c>
       <c r="G12">
         <f>SUM(G2:G11)</f>
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H12">
         <f>SUM(H2:H11)</f>
-        <v>-27</v>
+        <v>-33</v>
       </c>
       <c r="I12">
         <f>SUM(I2:I11)</f>
@@ -1331,7 +1332,7 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
@@ -1345,10 +1346,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F53"/>
+  <dimension ref="B1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1363,19 +1364,19 @@
     <row r="1" spans="2:6" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:6" ht="15.75" thickBot="1">
       <c r="B2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="2:6">
@@ -1383,10 +1384,10 @@
         <v>40428</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -1397,10 +1398,10 @@
         <v>40429</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1411,10 +1412,10 @@
         <v>40429</v>
       </c>
       <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
         <v>53</v>
-      </c>
-      <c r="D5" t="s">
-        <v>55</v>
       </c>
       <c r="F5">
         <v>1.5</v>
@@ -1425,10 +1426,10 @@
         <v>40431</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -1439,10 +1440,10 @@
         <v>40432</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F7">
         <v>4</v>
@@ -1453,10 +1454,10 @@
         <v>40432</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F8">
         <v>0.5</v>
@@ -1467,10 +1468,10 @@
         <v>40432</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F9">
         <v>2</v>
@@ -1481,10 +1482,10 @@
         <v>40432</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -1495,10 +1496,10 @@
         <v>40433</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F11">
         <v>6</v>
@@ -1506,7 +1507,7 @@
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -1518,13 +1519,13 @@
         <v>40435</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13">
         <v>3</v>
@@ -1535,10 +1536,10 @@
         <v>40435</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F14">
         <v>4</v>
@@ -1549,10 +1550,10 @@
         <v>40435</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F15">
         <v>1.5</v>
@@ -1563,10 +1564,10 @@
         <v>40435</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1577,10 +1578,10 @@
         <v>40435</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1591,10 +1592,10 @@
         <v>40435</v>
       </c>
       <c r="C18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" t="s">
         <v>64</v>
-      </c>
-      <c r="D18" t="s">
-        <v>66</v>
       </c>
       <c r="F18">
         <v>1.5</v>
@@ -1605,13 +1606,13 @@
         <v>40436</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F19">
         <v>2</v>
@@ -1622,13 +1623,13 @@
         <v>40436</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1639,10 +1640,10 @@
         <v>40436</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F21">
         <v>2</v>
@@ -1653,13 +1654,13 @@
         <v>40437</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F22">
         <v>2</v>
@@ -1670,13 +1671,13 @@
         <v>40438</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F23">
         <v>3</v>
@@ -1687,13 +1688,13 @@
         <v>40439</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F24">
         <v>5</v>
@@ -1704,10 +1705,10 @@
         <v>40439</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -1718,10 +1719,10 @@
         <v>40439</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1732,13 +1733,13 @@
         <v>40441</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F27">
         <v>4</v>
@@ -1749,13 +1750,13 @@
         <v>40442</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F28">
         <v>2</v>
@@ -1766,13 +1767,13 @@
         <v>40442</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F29">
         <v>2</v>
@@ -1783,10 +1784,10 @@
         <v>40442</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1797,10 +1798,10 @@
         <v>40442</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1811,10 +1812,10 @@
         <v>40444</v>
       </c>
       <c r="C32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F32">
         <v>0.5</v>
@@ -1825,10 +1826,10 @@
         <v>40444</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -1839,10 +1840,10 @@
         <v>40444</v>
       </c>
       <c r="C34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -1850,19 +1851,19 @@
     </row>
     <row r="35" spans="2:6">
       <c r="B35" s="1">
-        <v>40445</v>
+        <v>40444</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="E35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F35">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="2:6">
@@ -1870,13 +1871,16 @@
         <v>40445</v>
       </c>
       <c r="C36" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D36" t="s">
-        <v>75</v>
+        <v>60</v>
+      </c>
+      <c r="E36" t="s">
+        <v>13</v>
       </c>
       <c r="F36">
-        <v>0.25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="2:6">
@@ -1884,31 +1888,59 @@
         <v>40445</v>
       </c>
       <c r="C37" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D37" t="s">
-        <v>76</v>
-      </c>
-      <c r="E37" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F37">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" s="1">
+        <v>40445</v>
+      </c>
+      <c r="C38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:6">
-      <c r="B38" s="1"/>
-    </row>
-    <row r="53" spans="2:6">
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F53" s="3">
-        <f>SUM(F3:F52)</f>
-        <v>66.75</v>
+    <row r="39" spans="2:6">
+      <c r="B39" s="1">
+        <v>40445</v>
+      </c>
+      <c r="C39" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F54" s="3">
+        <f>SUM(F3:F53)</f>
+        <v>72.75</v>
       </c>
     </row>
   </sheetData>
@@ -1931,60 +1963,60 @@
   <sheetData>
     <row r="17" spans="2:4">
       <c r="C17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modificaciones en el indicador EV, arreglé algunos errores, hize el gráfico del indicador
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Earned Value" sheetId="1" r:id="rId1"/>
     <sheet name="Horas insumidas" sheetId="2" r:id="rId2"/>
     <sheet name="Estadísticas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="72">
   <si>
     <t>Id</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Hora Hombre</t>
-  </si>
-  <si>
     <t>Fecha</t>
   </si>
   <si>
@@ -138,36 +135,6 @@
     <t>ABM Campaña</t>
   </si>
   <si>
-    <t>Sem 1</t>
-  </si>
-  <si>
-    <t>Sem 2</t>
-  </si>
-  <si>
-    <t>Sem 3</t>
-  </si>
-  <si>
-    <t>Sem 4</t>
-  </si>
-  <si>
-    <t>Sem 5</t>
-  </si>
-  <si>
-    <t>Sem 6</t>
-  </si>
-  <si>
-    <t>Sem 7</t>
-  </si>
-  <si>
-    <t>Sem 8</t>
-  </si>
-  <si>
-    <t>Sem 9</t>
-  </si>
-  <si>
-    <t>Sem 10</t>
-  </si>
-  <si>
     <t>Crear arquitectura sistema</t>
   </si>
   <si>
@@ -247,13 +214,31 @@
   </si>
   <si>
     <t>% Avance esperado (0-50-100)</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Sprint 5</t>
+  </si>
+  <si>
+    <t>Sergio</t>
+  </si>
+  <si>
+    <t>Indicador EV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,8 +384,19 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="es-AR"/>
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -413,61 +409,197 @@
           <c:h val="0.8298611111111116"/>
         </c:manualLayout>
       </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:yVal>
+          <c:tx>
+            <c:strRef>
+              <c:f>Estadísticas!$C$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Estadísticas!$B$20:$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>'Earned Value'!$E$2:$E$11</c:f>
+              <c:f>Estadísticas!$C$20:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>60</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>20</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
+          </c:val>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="88480000"/>
-        <c:axId val="88485888"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="88480000"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Estadísticas!$D$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Estadísticas!$B$20:$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Estadísticas!$D$20:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Estadísticas!$E$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Estadísticas!$B$20:$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Estadísticas!$E$20:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="82062336"/>
+        <c:axId val="82134720"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="82062336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr rot="0" vert="horz"/>
@@ -483,33 +615,40 @@
                 <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88485888"/>
+        <c:crossAx val="82134720"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="88485888"/>
+        <c:axId val="82134720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88480000"/>
+        <c:crossAx val="82062336"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -631,6 +770,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -665,6 +805,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -840,14 +981,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="51.85546875" customWidth="1"/>
@@ -860,7 +1001,7 @@
     <col min="9" max="9" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -871,7 +1012,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -895,9 +1036,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -909,19 +1050,19 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <f>60*B15</f>
+        <f>60</f>
         <v>60</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A2,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
-        <v>30</v>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A2,'Horas insumidas'!$F$6:$F$129)</f>
+        <v>0</v>
       </c>
       <c r="H2">
         <f>F2-G2</f>
-        <v>-30</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <f>F2-E2</f>
@@ -931,53 +1072,53 @@
         <f>F2/E2</f>
         <v>0</v>
       </c>
-      <c r="K2">
+      <c r="K2" t="e">
         <f>F2/G2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D3">
         <v>100</v>
       </c>
       <c r="E3">
-        <f>40*B15</f>
+        <f>40</f>
         <v>40</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G3">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A3,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
-        <v>0</v>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A3,'Horas insumidas'!$F$6:$F$129)</f>
+        <v>33</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H11" si="0">F3-G3</f>
-        <v>0</v>
+        <f>F3-G3</f>
+        <v>7</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I11" si="1">F3-E3</f>
-        <v>-40</v>
+        <f>F3-E3</f>
+        <v>0</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J11" si="2">F3/E3</f>
-        <v>0</v>
-      </c>
-      <c r="K3" t="e">
-        <f t="shared" ref="K3:K11" si="3">F3/G3</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <f>F3/E3</f>
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <f>F3/G3</f>
+        <v>1.2121212121212122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -991,34 +1132,34 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <f>40*B15</f>
+        <f>40</f>
         <v>40</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A4,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
-        <v>3</v>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A4,'Horas insumidas'!$F$6:$F$129)</f>
+        <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
-        <v>-3</v>
+        <f t="shared" ref="H4:H11" si="0">F4-G4</f>
+        <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I4:I11" si="1">F4-E4</f>
         <v>-40</v>
       </c>
       <c r="J4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <f t="shared" ref="J4:J11" si="2">F4/E4</f>
+        <v>0</v>
+      </c>
+      <c r="K4" t="e">
+        <f t="shared" ref="K4:K11" si="3">F4/G4</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1032,14 +1173,14 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <f>40*B15</f>
+        <f>40</f>
         <v>40</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A5,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A5,'Horas insumidas'!$F$6:$F$129)</f>
         <v>0</v>
       </c>
       <c r="H5">
@@ -1059,7 +1200,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1073,14 +1214,14 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <f>40*B15</f>
+        <f>40</f>
         <v>40</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A6,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A6,'Horas insumidas'!$F$6:$F$129)</f>
         <v>0</v>
       </c>
       <c r="H6">
@@ -1100,7 +1241,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1114,14 +1255,14 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <f>40*B15</f>
+        <f>40</f>
         <v>40</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A7,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A7,'Horas insumidas'!$F$6:$F$129)</f>
         <v>0</v>
       </c>
       <c r="H7">
@@ -1141,7 +1282,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1155,14 +1296,14 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <f>20*B15</f>
+        <f>20</f>
         <v>20</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A8,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A8,'Horas insumidas'!$F$6:$F$129)</f>
         <v>0</v>
       </c>
       <c r="H8">
@@ -1182,7 +1323,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1196,14 +1337,14 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <f>20*B15</f>
+        <f>20</f>
         <v>20</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A9,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A9,'Horas insumidas'!$F$6:$F$129)</f>
         <v>0</v>
       </c>
       <c r="H9">
@@ -1223,7 +1364,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1237,14 +1378,14 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <f>40*B15</f>
+        <f>40</f>
         <v>40</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A10,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A10,'Horas insumidas'!$F$6:$F$129)</f>
         <v>0</v>
       </c>
       <c r="H10">
@@ -1264,7 +1405,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1278,14 +1419,14 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <f>20*B15</f>
+        <f>20</f>
         <v>20</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A11,'Horas insumidas'!$F$6:$F$129)*$B$15</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A11,'Horas insumidas'!$F$6:$F$129)</f>
         <v>0</v>
       </c>
       <c r="H11">
@@ -1305,7 +1446,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>32</v>
       </c>
@@ -1315,7 +1456,7 @@
       </c>
       <c r="F12">
         <f>SUM(F2:F11)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G12">
         <f>SUM(G2:G11)</f>
@@ -1323,20 +1464,15 @@
       </c>
       <c r="H12">
         <f>SUM(H2:H11)</f>
-        <v>-33</v>
+        <v>7</v>
       </c>
       <c r="I12">
         <f>SUM(I2:I11)</f>
-        <v>-360</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
+        <v>-320</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1345,14 +1481,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
@@ -1361,168 +1497,168 @@
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6">
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>40428</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>40429</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>40429</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F5">
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>40431</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>40432</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="F7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>40432</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F8">
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>40432</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>40432</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>40433</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="F11">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>40435</v>
       </c>
       <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
         <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>39</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
@@ -1531,85 +1667,85 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>40435</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F14">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>40435</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="F15">
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>40435</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>40435</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>40435</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="F18">
         <v>1.5</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>40436</v>
       </c>
       <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
         <v>38</v>
-      </c>
-      <c r="D19" t="s">
-        <v>39</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
@@ -1618,15 +1754,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>40436</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="E20" t="s">
         <v>13</v>
@@ -1635,29 +1771,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>40436</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="F21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>40437</v>
       </c>
       <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
         <v>38</v>
-      </c>
-      <c r="D22" t="s">
-        <v>39</v>
       </c>
       <c r="E22" t="s">
         <v>13</v>
@@ -1666,15 +1802,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>40438</v>
       </c>
       <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
         <v>38</v>
-      </c>
-      <c r="D23" t="s">
-        <v>39</v>
       </c>
       <c r="E23" t="s">
         <v>13</v>
@@ -1683,15 +1819,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>40439</v>
       </c>
       <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
         <v>38</v>
-      </c>
-      <c r="D24" t="s">
-        <v>39</v>
       </c>
       <c r="E24" t="s">
         <v>13</v>
@@ -1700,43 +1836,43 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>40439</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>40439</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>40441</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E27" t="s">
         <v>13</v>
@@ -1745,15 +1881,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>40442</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E28" t="s">
         <v>13</v>
@@ -1762,15 +1898,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>40442</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="E29" t="s">
         <v>13</v>
@@ -1779,85 +1915,85 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>40442</v>
       </c>
       <c r="C30" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D30" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:6">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>40442</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D31" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
         <v>40444</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D32" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="F32">
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="2:6">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
         <v>40444</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D33" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:6">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <v>40444</v>
       </c>
       <c r="C34" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D34" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:6">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <v>40444</v>
       </c>
       <c r="C35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" t="s">
         <v>38</v>
-      </c>
-      <c r="D35" t="s">
-        <v>39</v>
       </c>
       <c r="E35" t="s">
         <v>13</v>
@@ -1866,15 +2002,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="2:6">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <v>40445</v>
       </c>
       <c r="C36" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D36" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E36" t="s">
         <v>13</v>
@@ -1883,29 +2019,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>40445</v>
       </c>
       <c r="C37" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" t="s">
         <v>62</v>
-      </c>
-      <c r="D37" t="s">
-        <v>73</v>
       </c>
       <c r="F37">
         <v>0.25</v>
       </c>
     </row>
-    <row r="38" spans="2:6">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
         <v>40445</v>
       </c>
       <c r="C38" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D38" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="E38" t="s">
         <v>13</v>
@@ -1914,33 +2050,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:6">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>40445</v>
       </c>
       <c r="C39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" t="s">
         <v>38</v>
       </c>
-      <c r="D39" t="s">
-        <v>39</v>
-      </c>
       <c r="E39" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F39">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="2:6">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="1">
+        <v>40446</v>
+      </c>
+      <c r="C40" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" t="s">
+        <v>71</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="F54" s="3">
         <f>SUM(F3:F53)</f>
-        <v>72.75</v>
+        <v>73.75</v>
       </c>
     </row>
   </sheetData>
@@ -1954,69 +2104,108 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B17:D27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B19:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="17" spans="2:4">
-      <c r="C17" t="s">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
         <v>4</v>
       </c>
-      <c r="D17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" t="s">
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20">
+        <f>'Earned Value'!E3</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
+      <c r="D20">
+        <f>'Earned Value'!F3</f>
+        <v>40</v>
+      </c>
+      <c r="E20">
+        <f>'Earned Value'!G3</f>
+        <v>33</v>
+      </c>
+      <c r="F20">
+        <f>'Earned Value'!H3</f>
+        <v>7</v>
+      </c>
+      <c r="G20">
+        <f>'Earned Value'!I3</f>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f>'Earned Value'!J3</f>
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <f>'Earned Value'!K3</f>
+        <v>1.2121212121212122</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4">
+        <v>66</v>
+      </c>
+      <c r="C21">
+        <f>C20+40</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4">
+        <v>67</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22:C24" si="0">C21+40</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4">
+        <v>68</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="B25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27" t="s">
-        <v>49</v>
+        <v>69</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correccion del manual de configuracion
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Earned Value" sheetId="1" r:id="rId1"/>
     <sheet name="Horas insumidas" sheetId="2" r:id="rId2"/>
     <sheet name="Estadísticas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="114210"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="73">
   <si>
     <t>Id</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>Indicador EV</t>
+  </si>
+  <si>
+    <t>Correccion del Manual de Configuracion</t>
   </si>
 </sst>
 </file>
@@ -379,7 +382,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="es-AR"/>
   <c:chart>
     <c:plotArea>
       <c:layout>
@@ -387,10 +390,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.0833333333333331E-2"/>
+          <c:x val="7.0833333333333345E-2"/>
           <c:y val="4.8611111111111112E-2"/>
-          <c:w val="0.70416666666666672"/>
-          <c:h val="0.82986111111111116"/>
+          <c:w val="0.70416666666666661"/>
+          <c:h val="0.82986111111111127"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -558,11 +561,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="39606528"/>
-        <c:axId val="39616896"/>
+        <c:axId val="76333056"/>
+        <c:axId val="76334592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39606528"/>
+        <c:axId val="76333056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -583,17 +586,17 @@
                 <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39616896"/>
+        <c:crossAx val="76334592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39616896"/>
+        <c:axId val="76334592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -601,7 +604,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39606528"/>
+        <c:crossAx val="76333056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -614,8 +617,8 @@
           <c:yMode val="edge"/>
           <c:wMode val="edge"/>
           <c:hMode val="edge"/>
-          <c:x val="0.86875000000000002"/>
-          <c:y val="0.37152777777777779"/>
+          <c:x val="0.86875000000000013"/>
+          <c:y val="0.37152777777777796"/>
           <c:w val="0.98333333333333339"/>
           <c:h val="0.62152777777777779"/>
         </c:manualLayout>
@@ -626,7 +629,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -670,7 +673,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -956,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1029,7 +1032,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$129,A2,'Horas insumidas'!$F$6:$F$129)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A2,'Horas insumidas'!$F$6:$F$129)</f>
         <v>0</v>
       </c>
       <c r="H2">
@@ -1070,7 +1073,7 @@
         <v>40</v>
       </c>
       <c r="G3">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$129,A3,'Horas insumidas'!$F$6:$F$129)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A3,'Horas insumidas'!$F$6:$F$129)</f>
         <v>33.5</v>
       </c>
       <c r="H3">
@@ -1111,7 +1114,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$129,A4,'Horas insumidas'!$F$6:$F$129)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A4,'Horas insumidas'!$F$6:$F$129)</f>
         <v>0</v>
       </c>
       <c r="H4">
@@ -1152,7 +1155,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$129,A5,'Horas insumidas'!$F$6:$F$129)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A5,'Horas insumidas'!$F$6:$F$129)</f>
         <v>0</v>
       </c>
       <c r="H5">
@@ -1193,7 +1196,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$129,A6,'Horas insumidas'!$F$6:$F$129)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A6,'Horas insumidas'!$F$6:$F$129)</f>
         <v>0</v>
       </c>
       <c r="H6">
@@ -1234,7 +1237,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$129,A7,'Horas insumidas'!$F$6:$F$129)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A7,'Horas insumidas'!$F$6:$F$129)</f>
         <v>0</v>
       </c>
       <c r="H7">
@@ -1275,7 +1278,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$129,A8,'Horas insumidas'!$F$6:$F$129)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A8,'Horas insumidas'!$F$6:$F$129)</f>
         <v>0</v>
       </c>
       <c r="H8">
@@ -1316,7 +1319,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$129,A9,'Horas insumidas'!$F$6:$F$129)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A9,'Horas insumidas'!$F$6:$F$129)</f>
         <v>0</v>
       </c>
       <c r="H9">
@@ -1357,7 +1360,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$129,A10,'Horas insumidas'!$F$6:$F$129)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A10,'Horas insumidas'!$F$6:$F$129)</f>
         <v>0</v>
       </c>
       <c r="H10">
@@ -1398,7 +1401,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$129,A11,'Horas insumidas'!$F$6:$F$129)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$129,A11,'Horas insumidas'!$F$6:$F$129)</f>
         <v>0</v>
       </c>
       <c r="H11">
@@ -1456,15 +1459,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2053,6 +2056,20 @@
         <v>1</v>
       </c>
     </row>
+    <row r="41" spans="2:6">
+      <c r="B41" s="1">
+        <v>40448</v>
+      </c>
+      <c r="C41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" t="s">
+        <v>72</v>
+      </c>
+      <c r="F41">
+        <v>0.25</v>
+      </c>
+    </row>
     <row r="54" spans="2:6">
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -2062,7 +2079,7 @@
       </c>
       <c r="F54" s="3">
         <f>SUM(F3:F53)</f>
-        <v>74.25</v>
+        <v>74.5</v>
       </c>
     </row>
   </sheetData>
@@ -2116,31 +2133,31 @@
         <v>50</v>
       </c>
       <c r="C20">
-        <f ca="1">'Earned Value'!E3</f>
+        <f>'Earned Value'!E3</f>
         <v>40</v>
       </c>
       <c r="D20">
-        <f ca="1">'Earned Value'!F3</f>
+        <f>'Earned Value'!F3</f>
         <v>40</v>
       </c>
       <c r="E20">
-        <f ca="1">'Earned Value'!G3</f>
+        <f>'Earned Value'!G3</f>
         <v>33.5</v>
       </c>
       <c r="F20">
-        <f ca="1">'Earned Value'!H3</f>
+        <f>'Earned Value'!H3</f>
         <v>6.5</v>
       </c>
       <c r="G20">
-        <f ca="1">'Earned Value'!I3</f>
+        <f>'Earned Value'!I3</f>
         <v>0</v>
       </c>
       <c r="H20">
-        <f ca="1">'Earned Value'!J3</f>
+        <f>'Earned Value'!J3</f>
         <v>1</v>
       </c>
       <c r="I20">
-        <f ca="1">'Earned Value'!K3</f>
+        <f>'Earned Value'!K3</f>
         <v>1.1940298507462686</v>
       </c>
     </row>

</xml_diff>

<commit_message>
S-01018 - Se quita el campo codigo de la campaña, ya tenemos un campo Id
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Earned Value" sheetId="1" r:id="rId1"/>
     <sheet name="Horas insumidas" sheetId="2" r:id="rId2"/>
     <sheet name="Estadísticas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="114210"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="79">
   <si>
     <t>Id</t>
   </si>
@@ -198,9 +198,6 @@
     <t>Minuta de reunion</t>
   </si>
   <si>
-    <t>Total Sprint</t>
-  </si>
-  <si>
     <t>Creación de subtasks de stories</t>
   </si>
   <si>
@@ -241,6 +238,21 @@
   </si>
   <si>
     <t>Tareas de administracion para el primer Sprint</t>
+  </si>
+  <si>
+    <t>Scrolling en ABM de campaña</t>
+  </si>
+  <si>
+    <t>S-01018</t>
+  </si>
+  <si>
+    <t>Total Sprint 2</t>
+  </si>
+  <si>
+    <t>Total Sprint 1</t>
+  </si>
+  <si>
+    <t>Sacar campo codigo de la campaña</t>
   </si>
 </sst>
 </file>
@@ -388,7 +400,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="es-AR"/>
   <c:chart>
     <c:plotArea>
       <c:layout>
@@ -396,10 +408,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.0833333333333331E-2"/>
+          <c:x val="7.0833333333333373E-2"/>
           <c:y val="4.8611111111111112E-2"/>
-          <c:w val="0.70416666666666672"/>
-          <c:h val="0.82986111111111116"/>
+          <c:w val="0.7041666666666665"/>
+          <c:h val="0.82986111111111138"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -567,11 +579,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="39672064"/>
-        <c:axId val="39682432"/>
+        <c:axId val="55623680"/>
+        <c:axId val="55625216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39672064"/>
+        <c:axId val="55623680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -592,17 +604,17 @@
                 <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39682432"/>
+        <c:crossAx val="55625216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39682432"/>
+        <c:axId val="55625216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -610,7 +622,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39672064"/>
+        <c:crossAx val="55623680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -621,12 +633,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:wMode val="edge"/>
-          <c:hMode val="edge"/>
-          <c:x val="0.86875000000000002"/>
-          <c:y val="0.37152777777777779"/>
-          <c:w val="0.98333333333333339"/>
-          <c:h val="0.62152777777777779"/>
+          <c:x val="0.86875000000000024"/>
+          <c:y val="0.37152777777777807"/>
+          <c:w val="0.11458333333333325"/>
+          <c:h val="0.24999999999999989"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -635,7 +645,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -679,7 +689,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -965,7 +975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -993,7 +1003,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1038,7 +1048,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$117,A2,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A2,'Horas insumidas'!$F$6:$F$117)</f>
         <v>0</v>
       </c>
       <c r="H2">
@@ -1066,7 +1076,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>100</v>
@@ -1079,7 +1089,7 @@
         <v>40</v>
       </c>
       <c r="G3">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$117,A3,'Horas insumidas'!$F$6:$F$117)+SUMIF('Horas insumidas'!$E$6:$E$117,A12,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A3,'Horas insumidas'!$F$6:$F$117)+SUMIF('Horas insumidas'!$E$6:$E$117,A12,'Horas insumidas'!$F$6:$F$117)</f>
         <v>52.5</v>
       </c>
       <c r="H3">
@@ -1120,7 +1130,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$117,A4,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A4,'Horas insumidas'!$F$6:$F$117)</f>
         <v>0</v>
       </c>
       <c r="H4">
@@ -1161,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$117,A5,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A5,'Horas insumidas'!$F$6:$F$117)</f>
         <v>0</v>
       </c>
       <c r="H5">
@@ -1202,7 +1212,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$117,A6,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A6,'Horas insumidas'!$F$6:$F$117)</f>
         <v>0</v>
       </c>
       <c r="H6">
@@ -1243,7 +1253,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$117,A7,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A7,'Horas insumidas'!$F$6:$F$117)</f>
         <v>0</v>
       </c>
       <c r="H7">
@@ -1284,7 +1294,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$117,A8,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A8,'Horas insumidas'!$F$6:$F$117)</f>
         <v>0</v>
       </c>
       <c r="H8">
@@ -1325,7 +1335,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$117,A9,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A9,'Horas insumidas'!$F$6:$F$117)</f>
         <v>0</v>
       </c>
       <c r="H9">
@@ -1366,7 +1376,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$117,A10,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A10,'Horas insumidas'!$F$6:$F$117)</f>
         <v>0</v>
       </c>
       <c r="H10">
@@ -1407,7 +1417,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$117,A11,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A11,'Horas insumidas'!$F$6:$F$117)</f>
         <v>0</v>
       </c>
       <c r="H11">
@@ -1429,10 +1439,10 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
         <v>73</v>
-      </c>
-      <c r="B12" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1471,10 +1481,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F43"/>
+  <dimension ref="B1:F64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1667,7 +1677,7 @@
         <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F14">
         <v>4</v>
@@ -1684,7 +1694,7 @@
         <v>46</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F15">
         <v>1.5</v>
@@ -1701,7 +1711,7 @@
         <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1718,7 +1728,7 @@
         <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1735,7 +1745,7 @@
         <v>53</v>
       </c>
       <c r="E18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F18">
         <v>1.5</v>
@@ -1786,7 +1796,7 @@
         <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F21">
         <v>2</v>
@@ -1854,7 +1864,7 @@
         <v>45</v>
       </c>
       <c r="E25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -1871,7 +1881,7 @@
         <v>46</v>
       </c>
       <c r="E26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1939,7 +1949,7 @@
         <v>59</v>
       </c>
       <c r="E30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1956,7 +1966,7 @@
         <v>58</v>
       </c>
       <c r="E31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1973,7 +1983,7 @@
         <v>57</v>
       </c>
       <c r="E32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F32">
         <v>0.5</v>
@@ -1990,7 +2000,7 @@
         <v>45</v>
       </c>
       <c r="E33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -2004,10 +2014,10 @@
         <v>51</v>
       </c>
       <c r="D34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -2055,10 +2065,10 @@
         <v>51</v>
       </c>
       <c r="D37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F37">
         <v>0.25</v>
@@ -2072,7 +2082,7 @@
         <v>51</v>
       </c>
       <c r="D38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E38" t="s">
         <v>13</v>
@@ -2103,13 +2113,13 @@
         <v>40446</v>
       </c>
       <c r="C40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" t="s">
         <v>70</v>
       </c>
-      <c r="D40" t="s">
-        <v>71</v>
-      </c>
       <c r="E40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -2123,10 +2133,10 @@
         <v>51</v>
       </c>
       <c r="D41" t="s">
+        <v>71</v>
+      </c>
+      <c r="E41" t="s">
         <v>72</v>
-      </c>
-      <c r="E41" t="s">
-        <v>73</v>
       </c>
       <c r="F41">
         <v>0.25</v>
@@ -2137,7 +2147,7 @@
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="F42" s="3">
         <f>SUM(F3:F41)</f>
@@ -2146,12 +2156,58 @@
     </row>
     <row r="43" spans="2:6">
       <c r="B43" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="B44" s="1">
+        <v>40452</v>
+      </c>
+      <c r="C44" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" t="s">
+        <v>74</v>
+      </c>
+      <c r="E44" t="s">
+        <v>75</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="B45" s="1">
+        <v>40453</v>
+      </c>
+      <c r="C45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" t="s">
+        <v>78</v>
+      </c>
+      <c r="E45" t="s">
+        <v>75</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6">
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F64" s="3">
+        <f>SUM(F44:F63)</f>
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2205,37 +2261,37 @@
         <v>50</v>
       </c>
       <c r="C20">
-        <f ca="1">'Earned Value'!E3</f>
+        <f>'Earned Value'!E3</f>
         <v>40</v>
       </c>
       <c r="D20">
-        <f ca="1">'Earned Value'!F3</f>
+        <f>'Earned Value'!F3</f>
         <v>40</v>
       </c>
       <c r="E20">
-        <f ca="1">'Earned Value'!G3</f>
+        <f>'Earned Value'!G3</f>
         <v>52.5</v>
       </c>
       <c r="F20">
-        <f ca="1">'Earned Value'!H3</f>
+        <f>'Earned Value'!H3</f>
         <v>-12.5</v>
       </c>
       <c r="G20">
-        <f ca="1">'Earned Value'!I3</f>
+        <f>'Earned Value'!I3</f>
         <v>0</v>
       </c>
       <c r="H20">
-        <f ca="1">'Earned Value'!J3</f>
+        <f>'Earned Value'!J3</f>
         <v>1</v>
       </c>
       <c r="I20">
-        <f ca="1">'Earned Value'!K3</f>
+        <f>'Earned Value'!K3</f>
         <v>0.76190476190476186</v>
       </c>
     </row>
     <row r="21" spans="2:9">
       <c r="B21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21">
         <f>C20+40</f>
@@ -2244,7 +2300,7 @@
     </row>
     <row r="22" spans="2:9">
       <c r="B22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C22">
         <f>C21+40</f>
@@ -2253,7 +2309,7 @@
     </row>
     <row r="23" spans="2:9">
       <c r="B23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C23">
         <f>C22+40</f>
@@ -2262,7 +2318,7 @@
     </row>
     <row r="24" spans="2:9">
       <c r="B24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C24">
         <f>C23+40</f>

</xml_diff>

<commit_message>
S-01015: se cargan las horas insumidas para parsear el archivo HF.
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="81">
   <si>
     <t>Id</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t>Sacar campo codigo de la campaña</t>
+  </si>
+  <si>
+    <t>S-01015</t>
+  </si>
+  <si>
+    <t>Proceso archivo HF</t>
   </si>
 </sst>
 </file>
@@ -408,10 +414,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.0833333333333373E-2"/>
+          <c:x val="7.0833333333333387E-2"/>
           <c:y val="4.8611111111111112E-2"/>
           <c:w val="0.7041666666666665"/>
-          <c:h val="0.82986111111111138"/>
+          <c:h val="0.82986111111111149"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -579,11 +585,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="55623680"/>
-        <c:axId val="55625216"/>
+        <c:axId val="84303872"/>
+        <c:axId val="84305408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="55623680"/>
+        <c:axId val="84303872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -607,14 +613,14 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55625216"/>
+        <c:crossAx val="84305408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55625216"/>
+        <c:axId val="84305408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -622,7 +628,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55623680"/>
+        <c:crossAx val="84303872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -633,10 +639,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86875000000000024"/>
-          <c:y val="0.37152777777777807"/>
+          <c:x val="0.86875000000000036"/>
+          <c:y val="0.37152777777777818"/>
           <c:w val="0.11458333333333325"/>
-          <c:h val="0.24999999999999989"/>
+          <c:h val="0.24999999999999994"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -645,7 +651,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1048,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A2,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A2,'Horas insumidas'!$F$6:$F$118)</f>
         <v>0</v>
       </c>
       <c r="H2">
@@ -1089,7 +1095,7 @@
         <v>40</v>
       </c>
       <c r="G3">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A3,'Horas insumidas'!$F$6:$F$117)+SUMIF('Horas insumidas'!$E$6:$E$117,A12,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A3,'Horas insumidas'!$F$6:$F$118)+SUMIF('Horas insumidas'!$E$6:$E$118,A12,'Horas insumidas'!$F$6:$F$118)</f>
         <v>52.5</v>
       </c>
       <c r="H3">
@@ -1130,7 +1136,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A4,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A4,'Horas insumidas'!$F$6:$F$118)</f>
         <v>0</v>
       </c>
       <c r="H4">
@@ -1171,7 +1177,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A5,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A5,'Horas insumidas'!$F$6:$F$118)</f>
         <v>0</v>
       </c>
       <c r="H5">
@@ -1212,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A6,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A6,'Horas insumidas'!$F$6:$F$118)</f>
         <v>0</v>
       </c>
       <c r="H6">
@@ -1253,7 +1259,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A7,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A7,'Horas insumidas'!$F$6:$F$118)</f>
         <v>0</v>
       </c>
       <c r="H7">
@@ -1294,7 +1300,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A8,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A8,'Horas insumidas'!$F$6:$F$118)</f>
         <v>0</v>
       </c>
       <c r="H8">
@@ -1335,7 +1341,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A9,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A9,'Horas insumidas'!$F$6:$F$118)</f>
         <v>0</v>
       </c>
       <c r="H9">
@@ -1376,7 +1382,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A10,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A10,'Horas insumidas'!$F$6:$F$118)</f>
         <v>0</v>
       </c>
       <c r="H10">
@@ -1417,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$117,A11,'Horas insumidas'!$F$6:$F$117)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A11,'Horas insumidas'!$F$6:$F$118)</f>
         <v>0</v>
       </c>
       <c r="H11">
@@ -1481,10 +1487,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F64"/>
+  <dimension ref="B1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2165,47 +2171,64 @@
     </row>
     <row r="44" spans="2:6">
       <c r="B44" s="1">
-        <v>40452</v>
+        <v>40450</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D44" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E44" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="2:6">
       <c r="B45" s="1">
-        <v>40453</v>
+        <v>40452</v>
       </c>
       <c r="C45" t="s">
         <v>51</v>
       </c>
       <c r="D45" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E45" t="s">
         <v>75</v>
       </c>
       <c r="F45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="B46" s="1">
+        <v>40453</v>
+      </c>
+      <c r="C46" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" t="s">
+        <v>78</v>
+      </c>
+      <c r="E46" t="s">
+        <v>75</v>
+      </c>
+      <c r="F46">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="2:6">
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3" t="s">
+    <row r="65" spans="2:6">
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F64" s="3">
-        <f>SUM(F44:F63)</f>
+      <c r="F65" s="3">
+        <f>SUM(F45:F64)</f>
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
S-01018 _ Solucionado issue de minimo 1 metrica
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Earned Value" sheetId="1" r:id="rId1"/>
     <sheet name="Horas insumidas" sheetId="2" r:id="rId2"/>
     <sheet name="Estadísticas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="99">
   <si>
     <t>Id</t>
   </si>
@@ -301,6 +301,18 @@
   </si>
   <si>
     <t>Comenzada</t>
+  </si>
+  <si>
+    <t>Nacho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se modifico el hibernate.xml junto a los test y se resolvio el issue de </t>
+  </si>
+  <si>
+    <t>UAT Primer Sprint</t>
+  </si>
+  <si>
+    <t>Funcionalidad completa</t>
   </si>
 </sst>
 </file>
@@ -439,9 +451,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -449,6 +458,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -461,7 +473,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="es-AR"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:plotArea>
       <c:layout>
@@ -469,10 +481,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.0833333333333415E-2"/>
+          <c:x val="7.0140280561122245E-2"/>
           <c:y val="4.8611111111111112E-2"/>
-          <c:w val="0.7041666666666665"/>
-          <c:h val="0.8298611111111116"/>
+          <c:w val="0.70340681362725455"/>
+          <c:h val="0.82986111111111116"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -639,18 +651,18 @@
                   <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.5</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="35531392"/>
-        <c:axId val="35557760"/>
+        <c:axId val="39676160"/>
+        <c:axId val="39686528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="35531392"/>
+        <c:axId val="39676160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -671,17 +683,17 @@
                 <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35557760"/>
+        <c:crossAx val="39686528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35557760"/>
+        <c:axId val="39686528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -689,7 +701,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="35531392"/>
+        <c:crossAx val="39676160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -700,10 +712,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86875000000000058"/>
-          <c:y val="0.37152777777777829"/>
-          <c:w val="0.11458333333333325"/>
-          <c:h val="0.24999999999999997"/>
+          <c:x val="0.86773547094188375"/>
+          <c:y val="0.37152777777777779"/>
+          <c:w val="0.11422845691382766"/>
+          <c:h val="0.25"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -712,7 +724,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -756,7 +768,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1042,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1052,7 +1064,7 @@
     <col min="2" max="2" width="51.85546875" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" style="9" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" customWidth="1"/>
     <col min="8" max="8" width="6.5703125" customWidth="1"/>
@@ -1072,7 +1084,7 @@
       <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
@@ -1095,10 +1107,10 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>80</v>
       </c>
       <c r="C2" t="s">
@@ -1107,7 +1119,7 @@
       <c r="D2">
         <v>100</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="10">
         <f>40</f>
         <v>40</v>
       </c>
@@ -1115,7 +1127,7 @@
         <v>40</v>
       </c>
       <c r="G2">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A2,'Horas insumidas'!$F$6:$F$118)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$121,A2,'Horas insumidas'!$F$6:$F$121)</f>
         <v>33.5</v>
       </c>
       <c r="H2">
@@ -1136,10 +1148,10 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
@@ -1148,7 +1160,7 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="10">
         <f>40</f>
         <v>40</v>
       </c>
@@ -1156,7 +1168,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A3,'Horas insumidas'!$F$6:$F$118)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$121,A3,'Horas insumidas'!$F$6:$F$121)</f>
         <v>0</v>
       </c>
       <c r="H3">
@@ -1177,10 +1189,10 @@
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="s">
@@ -1189,7 +1201,7 @@
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <f>40</f>
         <v>40</v>
       </c>
@@ -1197,7 +1209,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A4,'Horas insumidas'!$F$6:$F$118)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$121,A4,'Horas insumidas'!$F$6:$F$121)</f>
         <v>0</v>
       </c>
       <c r="H4">
@@ -1218,10 +1230,10 @@
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C5" t="s">
@@ -1230,7 +1242,7 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <f>40</f>
         <v>40</v>
       </c>
@@ -1238,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A5,'Horas insumidas'!$F$6:$F$118)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$121,A5,'Horas insumidas'!$F$6:$F$121)</f>
         <v>0</v>
       </c>
       <c r="H5">
@@ -1259,10 +1271,10 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C6" t="s">
@@ -1271,7 +1283,7 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="10">
         <f>40</f>
         <v>40</v>
       </c>
@@ -1279,7 +1291,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A6,'Horas insumidas'!$F$6:$F$118)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$121,A6,'Horas insumidas'!$F$6:$F$121)</f>
         <v>0</v>
       </c>
       <c r="H6">
@@ -1300,10 +1312,10 @@
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C7" t="s">
@@ -1312,7 +1324,7 @@
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <f>20</f>
         <v>20</v>
       </c>
@@ -1320,7 +1332,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A7,'Horas insumidas'!$F$6:$F$118)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$121,A7,'Horas insumidas'!$F$6:$F$121)</f>
         <v>0</v>
       </c>
       <c r="H7">
@@ -1341,10 +1353,10 @@
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
@@ -1353,7 +1365,7 @@
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <f>20</f>
         <v>20</v>
       </c>
@@ -1361,7 +1373,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A8,'Horas insumidas'!$F$6:$F$118)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$121,A8,'Horas insumidas'!$F$6:$F$121)</f>
         <v>0</v>
       </c>
       <c r="H8">
@@ -1382,10 +1394,10 @@
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C9" t="s">
@@ -1394,7 +1406,7 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <f>40</f>
         <v>40</v>
       </c>
@@ -1402,7 +1414,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A9,'Horas insumidas'!$F$6:$F$118)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$121,A9,'Horas insumidas'!$F$6:$F$121)</f>
         <v>0</v>
       </c>
       <c r="H9">
@@ -1423,10 +1435,10 @@
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C10" t="s">
@@ -1435,7 +1447,7 @@
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="10">
         <f>20</f>
         <v>20</v>
       </c>
@@ -1443,7 +1455,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A10,'Horas insumidas'!$F$6:$F$118)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$121,A10,'Horas insumidas'!$F$6:$F$121)</f>
         <v>0</v>
       </c>
       <c r="H10">
@@ -1464,10 +1476,10 @@
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>82</v>
       </c>
       <c r="C11" t="s">
@@ -1476,7 +1488,7 @@
       <c r="D11">
         <v>0</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="10">
         <f>20</f>
         <v>20</v>
       </c>
@@ -1484,7 +1496,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A11,'Horas insumidas'!$F$6:$F$118)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$121,A11,'Horas insumidas'!$F$6:$F$121)</f>
         <v>0</v>
       </c>
       <c r="H11">
@@ -1505,10 +1517,10 @@
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>84</v>
       </c>
       <c r="C12" t="s">
@@ -1517,7 +1529,7 @@
       <c r="D12">
         <v>0</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="10">
         <f>20</f>
         <v>20</v>
       </c>
@@ -1525,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A12,'Horas insumidas'!$F$6:$F$118)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$121,A12,'Horas insumidas'!$F$6:$F$121)</f>
         <v>0</v>
       </c>
       <c r="H12">
@@ -1546,10 +1558,10 @@
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>86</v>
       </c>
       <c r="C13" t="s">
@@ -1558,7 +1570,7 @@
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="10">
         <f>20</f>
         <v>20</v>
       </c>
@@ -1566,7 +1578,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A13,'Horas insumidas'!$F$6:$F$118)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$121,A13,'Horas insumidas'!$F$6:$F$121)</f>
         <v>0</v>
       </c>
       <c r="H13">
@@ -1587,10 +1599,10 @@
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>88</v>
       </c>
       <c r="C14" t="s">
@@ -1599,7 +1611,7 @@
       <c r="D14">
         <v>0</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="10">
         <f>20</f>
         <v>20</v>
       </c>
@@ -1607,7 +1619,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A14,'Horas insumidas'!$F$6:$F$118)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$121,A14,'Horas insumidas'!$F$6:$F$121)</f>
         <v>0</v>
       </c>
       <c r="H14">
@@ -1628,10 +1640,10 @@
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>89</v>
       </c>
       <c r="C15" t="s">
@@ -1640,7 +1652,7 @@
       <c r="D15">
         <v>50</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="10">
         <f>20</f>
         <v>20</v>
       </c>
@@ -1648,12 +1660,12 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A15,'Horas insumidas'!$F$6:$F$118)</f>
-        <v>4</v>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$121,A15,'Horas insumidas'!$F$6:$F$121)</f>
+        <v>8</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>-8</v>
       </c>
       <c r="I15">
         <f t="shared" si="1"/>
@@ -1669,10 +1681,10 @@
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>91</v>
       </c>
       <c r="C16" t="s">
@@ -1681,7 +1693,7 @@
       <c r="D16">
         <v>0</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <f>20</f>
         <v>20</v>
       </c>
@@ -1689,7 +1701,7 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A16,'Horas insumidas'!$F$6:$F$118)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$121,A16,'Horas insumidas'!$F$6:$F$121)</f>
         <v>0</v>
       </c>
       <c r="H16">
@@ -1710,10 +1722,10 @@
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>93</v>
       </c>
       <c r="C17" t="s">
@@ -1722,7 +1734,7 @@
       <c r="D17">
         <v>0</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="10">
         <f>20</f>
         <v>20</v>
       </c>
@@ -1730,7 +1742,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A17,'Horas insumidas'!$F$6:$F$118)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$121,A17,'Horas insumidas'!$F$6:$F$121)</f>
         <v>0</v>
       </c>
       <c r="H17">
@@ -1751,10 +1763,10 @@
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C18" t="s">
@@ -1763,7 +1775,7 @@
       <c r="D18">
         <v>50</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="10">
         <f>13</f>
         <v>13</v>
       </c>
@@ -1771,12 +1783,12 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$118,A18,'Horas insumidas'!$F$6:$F$118)</f>
-        <v>13</v>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$121,A18,'Horas insumidas'!$F$6:$F$121)</f>
+        <v>16.5</v>
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
-        <v>-13</v>
+        <v>-16.5</v>
       </c>
       <c r="I18">
         <f t="shared" si="1"/>
@@ -1803,7 +1815,7 @@
       <c r="D20" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="9">
         <f>SUM(E2:E11)</f>
         <v>320</v>
       </c>
@@ -1835,10 +1847,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F65"/>
+  <dimension ref="B1:F68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1995,13 +2007,13 @@
       </c>
     </row>
     <row r="12" spans="2:6">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="1">
@@ -2509,13 +2521,13 @@
       </c>
     </row>
     <row r="43" spans="2:6">
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
     </row>
     <row r="44" spans="2:6">
       <c r="B44" s="1">
@@ -2536,16 +2548,16 @@
     </row>
     <row r="45" spans="2:6">
       <c r="B45" s="1">
-        <v>40452</v>
+        <v>40450</v>
       </c>
       <c r="C45" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D45" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="E45" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -2553,65 +2565,167 @@
     </row>
     <row r="46" spans="2:6">
       <c r="B46" s="1">
-        <v>40453</v>
+        <v>40450</v>
       </c>
       <c r="C46" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D46" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E46" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" ht="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6">
       <c r="B47" s="1">
-        <v>40452</v>
+        <v>40451</v>
       </c>
       <c r="C47" t="s">
-        <v>44</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>77</v>
+        <v>36</v>
+      </c>
+      <c r="D47" t="s">
+        <v>97</v>
       </c>
       <c r="E47" t="s">
         <v>71</v>
       </c>
       <c r="F47">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" ht="60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
       <c r="B48" s="1">
-        <v>40453</v>
+        <v>40452</v>
       </c>
       <c r="C48" t="s">
-        <v>44</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>78</v>
+        <v>47</v>
+      </c>
+      <c r="D48" t="s">
+        <v>70</v>
       </c>
       <c r="E48" t="s">
         <v>71</v>
       </c>
       <c r="F48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6">
+      <c r="B49" s="1">
+        <v>40453</v>
+      </c>
+      <c r="C49" t="s">
+        <v>47</v>
+      </c>
+      <c r="D49" t="s">
+        <v>74</v>
+      </c>
+      <c r="E49" t="s">
+        <v>71</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="30">
+      <c r="B50" s="1">
+        <v>40452</v>
+      </c>
+      <c r="C50" t="s">
+        <v>44</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E50" t="s">
+        <v>71</v>
+      </c>
+      <c r="F50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" ht="60">
+      <c r="B51" s="1">
+        <v>40453</v>
+      </c>
+      <c r="C51" t="s">
+        <v>44</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E51" t="s">
+        <v>71</v>
+      </c>
+      <c r="F51">
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="2:6">
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3" t="s">
+    <row r="52" spans="2:6" ht="18" customHeight="1">
+      <c r="B52" s="1">
+        <v>40454</v>
+      </c>
+      <c r="C52" t="s">
+        <v>95</v>
+      </c>
+      <c r="D52" t="s">
+        <v>96</v>
+      </c>
+      <c r="E52" t="s">
+        <v>71</v>
+      </c>
+      <c r="F52">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6">
+      <c r="B53" s="1">
+        <v>40454</v>
+      </c>
+      <c r="C53" t="s">
+        <v>36</v>
+      </c>
+      <c r="D53" t="s">
+        <v>53</v>
+      </c>
+      <c r="E53" t="s">
+        <v>75</v>
+      </c>
+      <c r="F53">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="B54" s="1">
+        <v>40454</v>
+      </c>
+      <c r="C54" t="s">
+        <v>36</v>
+      </c>
+      <c r="D54" t="s">
+        <v>98</v>
+      </c>
+      <c r="E54" t="s">
+        <v>75</v>
+      </c>
+      <c r="F54">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6">
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F65" s="3">
-        <f>SUM(F45:F64)</f>
-        <v>13</v>
+      <c r="F68" s="3">
+        <f>SUM(F48:F67)</f>
+        <v>17.5</v>
       </c>
     </row>
   </sheetData>
@@ -2629,8 +2743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B19:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2667,15 +2781,15 @@
         <v>46</v>
       </c>
       <c r="C20">
-        <f>'Earned Value'!E2</f>
+        <f ca="1">'Earned Value'!E2</f>
         <v>40</v>
       </c>
       <c r="D20">
-        <f>'Earned Value'!F2</f>
+        <f ca="1">'Earned Value'!F2</f>
         <v>40</v>
       </c>
       <c r="E20">
-        <f>'Earned Value'!G2</f>
+        <f ca="1">'Earned Value'!G2</f>
         <v>33.5</v>
       </c>
       <c r="F20">
@@ -2700,32 +2814,32 @@
         <v>61</v>
       </c>
       <c r="C21">
-        <f>C20+'Earned Value'!E15+'Earned Value'!E18</f>
+        <f ca="1">C20+'Earned Value'!E15+'Earned Value'!E18</f>
         <v>73</v>
       </c>
       <c r="D21">
-        <f>D20+'Earned Value'!F15+'Earned Value'!F18</f>
+        <f ca="1">D20+'Earned Value'!F15+'Earned Value'!F18</f>
         <v>40</v>
       </c>
       <c r="E21">
-        <f>E20+'Earned Value'!G15+'Earned Value'!G18</f>
-        <v>50.5</v>
+        <f ca="1">E20+'Earned Value'!G15+'Earned Value'!G18</f>
+        <v>58</v>
       </c>
       <c r="F21">
-        <f t="shared" ref="F21:F24" si="0">D21-E21</f>
-        <v>-10.5</v>
+        <f>D21-E21</f>
+        <v>-18</v>
       </c>
       <c r="G21">
-        <f t="shared" ref="G21:G24" si="1">D21-C21</f>
+        <f>D21-C21</f>
         <v>-33</v>
       </c>
       <c r="H21">
-        <f t="shared" ref="H21:H24" si="2">D21/C21</f>
+        <f>D21/C21</f>
         <v>0.54794520547945202</v>
       </c>
       <c r="I21">
-        <f t="shared" ref="I21:I24" si="3">D21/E21</f>
-        <v>0.79207920792079212</v>
+        <f>D21/E21</f>
+        <v>0.68965517241379315</v>
       </c>
     </row>
     <row r="22" spans="2:9">
@@ -2737,19 +2851,19 @@
         <v>113</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
+        <f>D22-E22</f>
         <v>0</v>
       </c>
       <c r="G22">
-        <f t="shared" si="1"/>
+        <f>D22-C22</f>
         <v>-113</v>
       </c>
       <c r="H22">
-        <f t="shared" si="2"/>
+        <f>D22/C22</f>
         <v>0</v>
       </c>
       <c r="I22" t="e">
-        <f t="shared" si="3"/>
+        <f>D22/E22</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2762,19 +2876,19 @@
         <v>153</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f>D23-E23</f>
         <v>0</v>
       </c>
       <c r="G23">
-        <f t="shared" si="1"/>
+        <f>D23-C23</f>
         <v>-153</v>
       </c>
       <c r="H23">
-        <f t="shared" si="2"/>
+        <f>D23/C23</f>
         <v>0</v>
       </c>
       <c r="I23" t="e">
-        <f t="shared" si="3"/>
+        <f>D23/E23</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2787,19 +2901,19 @@
         <v>193</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
+        <f>D24-E24</f>
         <v>0</v>
       </c>
       <c r="G24">
-        <f t="shared" si="1"/>
+        <f>D24-C24</f>
         <v>-193</v>
       </c>
       <c r="H24">
-        <f t="shared" si="2"/>
+        <f>D24/C24</f>
         <v>0</v>
       </c>
       <c r="I24" t="e">
-        <f t="shared" si="3"/>
+        <f>D24/E24</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
S-01004 - Avance en los datos de los graficos de performance de agentes
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Horas insumidas" sheetId="2" r:id="rId2"/>
     <sheet name="Estadísticas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="114210"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="109">
   <si>
     <t>Id</t>
   </si>
@@ -340,6 +340,9 @@
   </si>
   <si>
     <t>BC</t>
+  </si>
+  <si>
+    <t>Desarrollo Metricas Agentes</t>
   </si>
 </sst>
 </file>
@@ -500,7 +503,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="es-AR"/>
   <c:chart>
     <c:plotArea>
       <c:layout>
@@ -508,10 +511,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.0140280561122245E-2"/>
+          <c:x val="7.0140280561122259E-2"/>
           <c:y val="4.8611111111111112E-2"/>
           <c:w val="0.70340681362725455"/>
-          <c:h val="0.82986111111111116"/>
+          <c:h val="0.82986111111111138"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -685,11 +688,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="39676160"/>
-        <c:axId val="39690624"/>
+        <c:axId val="66183168"/>
+        <c:axId val="66184704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39676160"/>
+        <c:axId val="66183168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -710,17 +713,17 @@
                 <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39690624"/>
+        <c:crossAx val="66184704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39690624"/>
+        <c:axId val="66184704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -728,7 +731,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39676160"/>
+        <c:crossAx val="66183168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -741,9 +744,9 @@
           <c:yMode val="edge"/>
           <c:wMode val="edge"/>
           <c:hMode val="edge"/>
-          <c:x val="0.86773547094188375"/>
-          <c:y val="0.37152777777777779"/>
-          <c:w val="0.9819639278557114"/>
+          <c:x val="0.86773547094188408"/>
+          <c:y val="0.37152777777777807"/>
+          <c:w val="0.98196392785571118"/>
           <c:h val="0.62152777777777779"/>
         </c:manualLayout>
       </c:layout>
@@ -753,7 +756,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -797,7 +800,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1156,7 +1159,7 @@
         <v>40</v>
       </c>
       <c r="G2">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$131,A2,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A2,'Horas insumidas'!$F$6:$F$131)</f>
         <v>33.5</v>
       </c>
       <c r="H2">
@@ -1197,7 +1200,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$131,A3,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A3,'Horas insumidas'!$F$6:$F$131)</f>
         <v>0</v>
       </c>
       <c r="H3">
@@ -1238,12 +1241,12 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$131,A4,'Horas insumidas'!$F$6:$F$131)</f>
-        <v>8</v>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A4,'Horas insumidas'!$F$6:$F$131)</f>
+        <v>16</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H18" si="0">F4-G4</f>
-        <v>-8</v>
+        <v>-16</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I18" si="1">F4-E4</f>
@@ -1279,7 +1282,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$131,A5,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A5,'Horas insumidas'!$F$6:$F$131)</f>
         <v>0</v>
       </c>
       <c r="H5">
@@ -1320,7 +1323,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$131,A6,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A6,'Horas insumidas'!$F$6:$F$131)</f>
         <v>0</v>
       </c>
       <c r="H6">
@@ -1361,7 +1364,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$131,A7,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A7,'Horas insumidas'!$F$6:$F$131)</f>
         <v>21</v>
       </c>
       <c r="H7">
@@ -1402,7 +1405,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$131,A8,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A8,'Horas insumidas'!$F$6:$F$131)</f>
         <v>0</v>
       </c>
       <c r="H8">
@@ -1443,7 +1446,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$131,A9,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A9,'Horas insumidas'!$F$6:$F$131)</f>
         <v>0</v>
       </c>
       <c r="H9">
@@ -1484,7 +1487,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$131,A10,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A10,'Horas insumidas'!$F$6:$F$131)</f>
         <v>0</v>
       </c>
       <c r="H10">
@@ -1525,7 +1528,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$131,A11,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A11,'Horas insumidas'!$F$6:$F$131)</f>
         <v>0</v>
       </c>
       <c r="H11">
@@ -1566,7 +1569,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$131,A12,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A12,'Horas insumidas'!$F$6:$F$131)</f>
         <v>5</v>
       </c>
       <c r="H12">
@@ -1607,7 +1610,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$131,A13,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A13,'Horas insumidas'!$F$6:$F$131)</f>
         <v>0</v>
       </c>
       <c r="H13">
@@ -1648,7 +1651,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$131,A14,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A14,'Horas insumidas'!$F$6:$F$131)</f>
         <v>0</v>
       </c>
       <c r="H14">
@@ -1689,7 +1692,7 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$131,A15,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A15,'Horas insumidas'!$F$6:$F$131)</f>
         <v>8</v>
       </c>
       <c r="H15">
@@ -1730,7 +1733,7 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$131,A16,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A16,'Horas insumidas'!$F$6:$F$131)</f>
         <v>0</v>
       </c>
       <c r="H16">
@@ -1771,7 +1774,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$131,A17,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A17,'Horas insumidas'!$F$6:$F$131)</f>
         <v>0</v>
       </c>
       <c r="H17">
@@ -1812,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$131,A18,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A18,'Horas insumidas'!$F$6:$F$131)</f>
         <v>17.5</v>
       </c>
       <c r="H18">
@@ -1862,11 +1865,11 @@
       </c>
       <c r="G21">
         <f>SUM(G2:G11)</f>
-        <v>62.5</v>
+        <v>70.5</v>
       </c>
       <c r="H21">
         <f>SUM(H2:H11)</f>
-        <v>-22.5</v>
+        <v>-30.5</v>
       </c>
       <c r="I21">
         <f>SUM(I2:I18)</f>
@@ -1886,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2976,7 +2979,7 @@
     </row>
     <row r="68" spans="2:6">
       <c r="B68" s="1">
-        <v>40468</v>
+        <v>40465</v>
       </c>
       <c r="C68" t="s">
         <v>36</v>
@@ -2993,7 +2996,7 @@
     </row>
     <row r="69" spans="2:6">
       <c r="B69" s="1">
-        <v>40468</v>
+        <v>40465</v>
       </c>
       <c r="C69" t="s">
         <v>36</v>
@@ -3006,6 +3009,40 @@
       </c>
       <c r="F69">
         <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6">
+      <c r="B70" s="1">
+        <v>40465</v>
+      </c>
+      <c r="C70" t="s">
+        <v>47</v>
+      </c>
+      <c r="D70" t="s">
+        <v>108</v>
+      </c>
+      <c r="E70" t="s">
+        <v>14</v>
+      </c>
+      <c r="F70">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6">
+      <c r="B71" s="1">
+        <v>40466</v>
+      </c>
+      <c r="C71" t="s">
+        <v>47</v>
+      </c>
+      <c r="D71" t="s">
+        <v>108</v>
+      </c>
+      <c r="E71" t="s">
+        <v>14</v>
+      </c>
+      <c r="F71">
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -3017,7 +3054,7 @@
       </c>
       <c r="F78" s="3">
         <f>SUM(F48:F77)</f>
-        <v>57.5</v>
+        <v>65.5</v>
       </c>
     </row>
   </sheetData>
@@ -3073,15 +3110,15 @@
         <v>46</v>
       </c>
       <c r="C20">
-        <f ca="1">'Earned Value'!E2</f>
+        <f>'Earned Value'!E2</f>
         <v>40</v>
       </c>
       <c r="D20">
-        <f ca="1">'Earned Value'!F2</f>
+        <f>'Earned Value'!F2</f>
         <v>40</v>
       </c>
       <c r="E20">
-        <f ca="1">'Earned Value'!G2</f>
+        <f>'Earned Value'!G2</f>
         <v>33.5</v>
       </c>
       <c r="F20">
@@ -3109,11 +3146,11 @@
         <v>93</v>
       </c>
       <c r="D21">
-        <f ca="1">D20+'Earned Value'!F15+'Earned Value'!F18</f>
+        <f>D20+'Earned Value'!F15+'Earned Value'!F18</f>
         <v>40</v>
       </c>
       <c r="E21">
-        <f ca="1">E20+'Earned Value'!G15+'Earned Value'!G18</f>
+        <f>E20+'Earned Value'!G15+'Earned Value'!G18</f>
         <v>59</v>
       </c>
       <c r="F21">

</xml_diff>

<commit_message>
S-01020 - Se agregan metricas y se linkea el calculo de la metrica QA_PTS_POSSIBLE con el grafico
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="114">
   <si>
     <t>Id</t>
   </si>
@@ -348,7 +348,16 @@
     <t>Desarrollo métrica AUX_TM</t>
   </si>
   <si>
-    <t>TK-01035</t>
+    <t>TK-01036</t>
+  </si>
+  <si>
+    <t>Desarrollo metrica QA_PTS_POSSIBLE</t>
+  </si>
+  <si>
+    <t>S-01020</t>
+  </si>
+  <si>
+    <t>Framework de metricas y graficos</t>
   </si>
 </sst>
 </file>
@@ -694,11 +703,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="66001152"/>
-        <c:axId val="110510848"/>
+        <c:axId val="72278016"/>
+        <c:axId val="72279552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66001152"/>
+        <c:axId val="72278016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -722,14 +731,14 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110510848"/>
+        <c:crossAx val="72279552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110510848"/>
+        <c:axId val="72279552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -737,7 +746,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66001152"/>
+        <c:crossAx val="72278016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -750,9 +759,9 @@
           <c:yMode val="edge"/>
           <c:wMode val="edge"/>
           <c:hMode val="edge"/>
-          <c:x val="0.86773547094188452"/>
-          <c:y val="0.37152777777777829"/>
-          <c:w val="0.98196392785571096"/>
+          <c:x val="0.86773547094188475"/>
+          <c:y val="0.37152777777777846"/>
+          <c:w val="0.98196392785571085"/>
           <c:h val="0.62152777777777779"/>
         </c:manualLayout>
       </c:layout>
@@ -762,7 +771,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1893,10 +1902,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F82"/>
+  <dimension ref="B1:F84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3091,19 +3100,53 @@
     </row>
     <row r="82" spans="2:6">
       <c r="B82" s="1">
+        <v>40471</v>
+      </c>
+      <c r="C82" t="s">
+        <v>47</v>
+      </c>
+      <c r="D82" t="s">
+        <v>111</v>
+      </c>
+      <c r="E82" t="s">
+        <v>112</v>
+      </c>
+      <c r="F82">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6">
+      <c r="B83" s="1">
         <v>40472</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C83" t="s">
         <v>33</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D83" t="s">
         <v>109</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E83" t="s">
         <v>110</v>
       </c>
-      <c r="F82">
+      <c r="F83">
         <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6">
+      <c r="B84" s="1">
+        <v>40472</v>
+      </c>
+      <c r="C84" t="s">
+        <v>47</v>
+      </c>
+      <c r="D84" t="s">
+        <v>113</v>
+      </c>
+      <c r="E84" t="s">
+        <v>112</v>
+      </c>
+      <c r="F84">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
S-01020 - horas tests métricas QA.
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="116">
   <si>
     <t>Id</t>
   </si>
@@ -361,6 +361,9 @@
   </si>
   <si>
     <t>Mostrando las métricas por pantalla</t>
+  </si>
+  <si>
+    <t>Tests métricas QA</t>
   </si>
 </sst>
 </file>
@@ -706,11 +709,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="43578112"/>
-        <c:axId val="43579648"/>
+        <c:axId val="44565248"/>
+        <c:axId val="44566784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="43578112"/>
+        <c:axId val="44565248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -734,14 +737,14 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43579648"/>
+        <c:crossAx val="44566784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43579648"/>
+        <c:axId val="44566784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -749,7 +752,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43578112"/>
+        <c:crossAx val="44565248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -762,9 +765,9 @@
           <c:yMode val="edge"/>
           <c:wMode val="edge"/>
           <c:hMode val="edge"/>
-          <c:x val="0.86773547094188486"/>
-          <c:y val="0.37152777777777857"/>
-          <c:w val="0.98196392785571063"/>
+          <c:x val="0.86773547094188508"/>
+          <c:y val="0.37152777777777868"/>
+          <c:w val="0.98196392785571041"/>
           <c:h val="0.62152777777777779"/>
         </c:manualLayout>
       </c:layout>
@@ -774,7 +777,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1905,10 +1908,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F85"/>
+  <dimension ref="B1:F86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3167,6 +3170,23 @@
       </c>
       <c r="F85">
         <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6">
+      <c r="B86" s="1">
+        <v>40474</v>
+      </c>
+      <c r="C86" t="s">
+        <v>33</v>
+      </c>
+      <c r="D86" t="s">
+        <v>115</v>
+      </c>
+      <c r="E86" t="s">
+        <v>112</v>
+      </c>
+      <c r="F86">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
S-01020 - se agrega fecha desde y fecha hasta a las métricas.
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Earned Value" sheetId="1" r:id="rId1"/>
     <sheet name="Horas insumidas" sheetId="2" r:id="rId2"/>
     <sheet name="Estadísticas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="114210"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="125">
   <si>
     <t>Id</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t>Total Sprint 3</t>
+  </si>
+  <si>
+    <t>Se agrego rango de fechas a la métricas</t>
   </si>
 </sst>
 </file>
@@ -549,7 +552,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="es-AR"/>
   <c:chart>
     <c:plotArea>
       <c:layout>
@@ -557,10 +560,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.0140280561122245E-2"/>
+          <c:x val="7.0140280561122259E-2"/>
           <c:y val="4.8611111111111112E-2"/>
           <c:w val="0.70340681362725455"/>
-          <c:h val="0.82986111111111116"/>
+          <c:h val="0.82986111111111127"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -740,11 +743,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="39676160"/>
-        <c:axId val="39690624"/>
+        <c:axId val="80109568"/>
+        <c:axId val="80111104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39676160"/>
+        <c:axId val="80109568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -765,17 +768,17 @@
                 <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39690624"/>
+        <c:crossAx val="80111104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39690624"/>
+        <c:axId val="80111104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -783,7 +786,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39676160"/>
+        <c:crossAx val="80109568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -794,12 +797,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:wMode val="edge"/>
-          <c:hMode val="edge"/>
-          <c:x val="0.86773547094188375"/>
-          <c:y val="0.37152777777777779"/>
-          <c:w val="0.9819639278557114"/>
-          <c:h val="0.62152777777777779"/>
+          <c:x val="0.86773547094188386"/>
+          <c:y val="0.37152777777777796"/>
+          <c:w val="0.11422845691382744"/>
+          <c:h val="0.24999999999999983"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -808,7 +809,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -852,7 +853,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1211,7 +1212,7 @@
         <v>40</v>
       </c>
       <c r="G2">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A2,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A2,'Horas insumidas'!$F$6:$F$135)</f>
         <v>33.5</v>
       </c>
       <c r="H2">
@@ -1252,7 +1253,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A3,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A3,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H3">
@@ -1293,7 +1294,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A4,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A4,'Horas insumidas'!$F$6:$F$135)</f>
         <v>17</v>
       </c>
       <c r="H4">
@@ -1334,7 +1335,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A5,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A5,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H5">
@@ -1375,7 +1376,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A6,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A6,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H6">
@@ -1416,7 +1417,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A7,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A7,'Horas insumidas'!$F$6:$F$135)</f>
         <v>21</v>
       </c>
       <c r="H7">
@@ -1457,7 +1458,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A8,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A8,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H8">
@@ -1498,7 +1499,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A9,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A9,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H9">
@@ -1539,7 +1540,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A10,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A10,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H10">
@@ -1580,7 +1581,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A11,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A11,'Horas insumidas'!$F$6:$F$135)</f>
         <v>3.5</v>
       </c>
       <c r="H11">
@@ -1621,7 +1622,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A12,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A12,'Horas insumidas'!$F$6:$F$135)</f>
         <v>5</v>
       </c>
       <c r="H12">
@@ -1662,7 +1663,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A13,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A13,'Horas insumidas'!$F$6:$F$135)</f>
         <v>4.5</v>
       </c>
       <c r="H13">
@@ -1703,7 +1704,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A14,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A14,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H14">
@@ -1744,7 +1745,7 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A15,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A15,'Horas insumidas'!$F$6:$F$135)</f>
         <v>8</v>
       </c>
       <c r="H15">
@@ -1785,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A16,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A16,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H16">
@@ -1826,7 +1827,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A17,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A17,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H17">
@@ -1867,7 +1868,7 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A18,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A18,'Horas insumidas'!$F$6:$F$135)</f>
         <v>17.5</v>
       </c>
       <c r="H18">
@@ -1907,12 +1908,12 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A19,'Horas insumidas'!$F$6:$F$135)</f>
-        <v>18</v>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A19,'Horas insumidas'!$F$6:$F$135)</f>
+        <v>21</v>
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>-18</v>
+        <v>-21</v>
       </c>
       <c r="I19">
         <f t="shared" si="1"/>
@@ -1947,7 +1948,7 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A20,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A20,'Horas insumidas'!$F$6:$F$135)</f>
         <v>1</v>
       </c>
       <c r="H20">
@@ -2005,11 +2006,11 @@
       </c>
       <c r="G24">
         <f>SUM(G2:G20)</f>
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H24">
         <f>SUM(H2:H20)</f>
-        <v>-89</v>
+        <v>-92</v>
       </c>
       <c r="I24">
         <f>SUM(I2:I20)</f>
@@ -2029,8 +2030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F110"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="F94" sqref="F94"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3427,6 +3428,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="94" spans="2:6">
+      <c r="B94" s="1">
+        <v>40475</v>
+      </c>
+      <c r="C94" t="s">
+        <v>33</v>
+      </c>
+      <c r="D94" t="s">
+        <v>124</v>
+      </c>
+      <c r="E94" t="s">
+        <v>112</v>
+      </c>
+      <c r="F94">
+        <v>3</v>
+      </c>
+    </row>
     <row r="110" spans="2:6">
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -3436,7 +3454,7 @@
       </c>
       <c r="F110" s="3">
         <f>SUM(F80:F109)</f>
-        <v>33.5</v>
+        <v>36.5</v>
       </c>
     </row>
   </sheetData>
@@ -3455,7 +3473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B19:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -3493,15 +3511,15 @@
         <v>46</v>
       </c>
       <c r="C20">
-        <f ca="1">'Earned Value'!E2</f>
+        <f>'Earned Value'!E2</f>
         <v>40</v>
       </c>
       <c r="D20">
-        <f ca="1">'Earned Value'!F2</f>
+        <f>'Earned Value'!F2</f>
         <v>40</v>
       </c>
       <c r="E20">
-        <f ca="1">'Earned Value'!G2</f>
+        <f>'Earned Value'!G2</f>
         <v>33.5</v>
       </c>
       <c r="F20">

</xml_diff>

<commit_message>
S-01020 - horas Duilio.
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="126">
   <si>
     <t>Id</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>Se agrego rango de fechas a la métricas</t>
+  </si>
+  <si>
+    <t>Se cargaron datos de prueba y se corrigieron los tests</t>
   </si>
 </sst>
 </file>
@@ -563,7 +566,7 @@
           <c:x val="7.0140280561122259E-2"/>
           <c:y val="4.8611111111111112E-2"/>
           <c:w val="0.70340681362725455"/>
-          <c:h val="0.82986111111111127"/>
+          <c:h val="0.82986111111111138"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -743,11 +746,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="80109568"/>
-        <c:axId val="80111104"/>
+        <c:axId val="80101376"/>
+        <c:axId val="80102912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80109568"/>
+        <c:axId val="80101376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -771,14 +774,14 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80111104"/>
+        <c:crossAx val="80102912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80111104"/>
+        <c:axId val="80102912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -786,7 +789,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80109568"/>
+        <c:crossAx val="80101376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -797,10 +800,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86773547094188386"/>
-          <c:y val="0.37152777777777796"/>
-          <c:w val="0.11422845691382744"/>
-          <c:h val="0.24999999999999983"/>
+          <c:x val="0.86773547094188408"/>
+          <c:y val="0.37152777777777807"/>
+          <c:w val="0.11422845691382745"/>
+          <c:h val="0.24999999999999989"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -809,7 +812,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1909,11 +1912,11 @@
       </c>
       <c r="G19">
         <f>SUMIF('Horas insumidas'!$E$6:$E$135,A19,'Horas insumidas'!$F$6:$F$135)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>-21</v>
+        <v>-23</v>
       </c>
       <c r="I19">
         <f t="shared" si="1"/>
@@ -2006,11 +2009,11 @@
       </c>
       <c r="G24">
         <f>SUM(G2:G20)</f>
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H24">
         <f>SUM(H2:H20)</f>
-        <v>-92</v>
+        <v>-94</v>
       </c>
       <c r="I24">
         <f>SUM(I2:I20)</f>
@@ -2031,7 +2034,7 @@
   <dimension ref="B1:F110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3445,6 +3448,23 @@
         <v>3</v>
       </c>
     </row>
+    <row r="95" spans="2:6">
+      <c r="B95" s="1">
+        <v>40475</v>
+      </c>
+      <c r="C95" t="s">
+        <v>33</v>
+      </c>
+      <c r="D95" t="s">
+        <v>125</v>
+      </c>
+      <c r="E95" t="s">
+        <v>112</v>
+      </c>
+      <c r="F95">
+        <v>2</v>
+      </c>
+    </row>
     <row r="110" spans="2:6">
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -3454,7 +3474,7 @@
       </c>
       <c r="F110" s="3">
         <f>SUM(F80:F109)</f>
-        <v>36.5</v>
+        <v>38.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TK-01036 - Métrica AVG_TALK_TM
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="127">
   <si>
     <t>Id</t>
   </si>
@@ -394,6 +394,9 @@
   </si>
   <si>
     <t>Se cargaron datos de prueba y se corrigieron los tests</t>
+  </si>
+  <si>
+    <t>Métrica AVG_TALK_TM</t>
   </si>
 </sst>
 </file>
@@ -566,7 +569,7 @@
           <c:x val="7.0140280561122259E-2"/>
           <c:y val="4.8611111111111112E-2"/>
           <c:w val="0.70340681362725455"/>
-          <c:h val="0.82986111111111138"/>
+          <c:h val="0.82986111111111149"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -746,11 +749,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="80101376"/>
-        <c:axId val="80102912"/>
+        <c:axId val="83189760"/>
+        <c:axId val="83191296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80101376"/>
+        <c:axId val="83189760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -774,14 +777,14 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80102912"/>
+        <c:crossAx val="83191296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80102912"/>
+        <c:axId val="83191296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -789,7 +792,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80101376"/>
+        <c:crossAx val="83189760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -800,10 +803,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86773547094188408"/>
-          <c:y val="0.37152777777777807"/>
-          <c:w val="0.11422845691382745"/>
-          <c:h val="0.24999999999999989"/>
+          <c:x val="0.8677354709418843"/>
+          <c:y val="0.37152777777777818"/>
+          <c:w val="0.11422845691382746"/>
+          <c:h val="0.24999999999999994"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -812,7 +815,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2034,7 +2037,7 @@
   <dimension ref="B1:F110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+      <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3465,6 +3468,23 @@
         <v>2</v>
       </c>
     </row>
+    <row r="96" spans="2:6">
+      <c r="B96" s="1">
+        <v>40475</v>
+      </c>
+      <c r="C96" t="s">
+        <v>33</v>
+      </c>
+      <c r="D96" t="s">
+        <v>126</v>
+      </c>
+      <c r="E96" t="s">
+        <v>110</v>
+      </c>
+      <c r="F96">
+        <v>3</v>
+      </c>
+    </row>
     <row r="110" spans="2:6">
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -3474,7 +3494,7 @@
       </c>
       <c r="F110" s="3">
         <f>SUM(F80:F109)</f>
-        <v>38.5</v>
+        <v>41.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
S-01021 - Se modifica el formato de la pantalla visualizar sueldo.
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="129">
   <si>
     <t>Id</t>
   </si>
@@ -397,6 +397,12 @@
   </si>
   <si>
     <t>Métrica AVG_TALK_TM</t>
+  </si>
+  <si>
+    <t>S-01021</t>
+  </si>
+  <si>
+    <t>Se modifica pantalla para mostrar las métricas de un agente</t>
   </si>
 </sst>
 </file>
@@ -569,7 +575,7 @@
           <c:x val="7.0140280561122259E-2"/>
           <c:y val="4.8611111111111112E-2"/>
           <c:w val="0.70340681362725455"/>
-          <c:h val="0.82986111111111149"/>
+          <c:h val="0.8298611111111116"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -803,10 +809,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.8677354709418843"/>
-          <c:y val="0.37152777777777818"/>
+          <c:x val="0.86773547094188452"/>
+          <c:y val="0.37152777777777829"/>
           <c:w val="0.11422845691382746"/>
-          <c:h val="0.24999999999999994"/>
+          <c:h val="0.24999999999999997"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -815,7 +821,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000389" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000389" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2037,7 +2043,7 @@
   <dimension ref="B1:F110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="F97" sqref="F97"/>
+      <selection activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3485,6 +3491,23 @@
         <v>3</v>
       </c>
     </row>
+    <row r="97" spans="2:6">
+      <c r="B97" s="1">
+        <v>40475</v>
+      </c>
+      <c r="C97" t="s">
+        <v>33</v>
+      </c>
+      <c r="D97" t="s">
+        <v>128</v>
+      </c>
+      <c r="E97" t="s">
+        <v>127</v>
+      </c>
+      <c r="F97">
+        <v>1</v>
+      </c>
+    </row>
     <row r="110" spans="2:6">
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -3494,7 +3517,7 @@
       </c>
       <c r="F110" s="3">
         <f>SUM(F80:F109)</f>
-        <v>41.5</v>
+        <v>42.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
S-01022 - horas duilio.
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="130">
   <si>
     <t>Id</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>Se modifica pantalla para mostrar las métricas de un agente</t>
+  </si>
+  <si>
+    <t>Se corrige bug al agregar un supervisor a la campaña</t>
   </si>
 </sst>
 </file>
@@ -755,11 +758,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="83189760"/>
-        <c:axId val="83191296"/>
+        <c:axId val="66000000"/>
+        <c:axId val="66001536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83189760"/>
+        <c:axId val="66000000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -783,14 +786,14 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83191296"/>
+        <c:crossAx val="66001536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83191296"/>
+        <c:axId val="66001536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -798,7 +801,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83189760"/>
+        <c:crossAx val="66000000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -809,10 +812,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86773547094188452"/>
-          <c:y val="0.37152777777777829"/>
+          <c:x val="0.86773547094188475"/>
+          <c:y val="0.37152777777777846"/>
           <c:w val="0.11422845691382746"/>
-          <c:h val="0.24999999999999997"/>
+          <c:h val="0.25"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -821,7 +824,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000389" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000389" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000004" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000004" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1961,11 +1964,11 @@
       </c>
       <c r="G20">
         <f>SUMIF('Horas insumidas'!$E$6:$E$135,A20,'Horas insumidas'!$F$6:$F$135)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="I20">
         <f t="shared" si="1"/>
@@ -2018,11 +2021,11 @@
       </c>
       <c r="G24">
         <f>SUM(G2:G20)</f>
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H24">
         <f>SUM(H2:H20)</f>
-        <v>-94</v>
+        <v>-95</v>
       </c>
       <c r="I24">
         <f>SUM(I2:I20)</f>
@@ -2043,7 +2046,7 @@
   <dimension ref="B1:F110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="F98" sqref="F98"/>
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3508,6 +3511,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="98" spans="2:6">
+      <c r="B98" s="1">
+        <v>40476</v>
+      </c>
+      <c r="C98" t="s">
+        <v>33</v>
+      </c>
+      <c r="D98" t="s">
+        <v>129</v>
+      </c>
+      <c r="E98" t="s">
+        <v>119</v>
+      </c>
+      <c r="F98">
+        <v>1</v>
+      </c>
+    </row>
     <row r="110" spans="2:6">
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -3517,7 +3537,7 @@
       </c>
       <c r="F110" s="3">
         <f>SUM(F80:F109)</f>
-        <v>42.5</v>
+        <v>43.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
S-01020 - Métrica AUX_TM
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Earned Value" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="131">
   <si>
     <t>Id</t>
   </si>
@@ -406,6 +406,9 @@
   </si>
   <si>
     <t>Se corrige bug al agregar un supervisor a la campaña</t>
+  </si>
+  <si>
+    <t>Métrica AUX_TM</t>
   </si>
 </sst>
 </file>
@@ -758,11 +761,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="66000000"/>
-        <c:axId val="66001536"/>
+        <c:axId val="80109568"/>
+        <c:axId val="80111104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66000000"/>
+        <c:axId val="80109568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -786,14 +789,14 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66001536"/>
+        <c:crossAx val="80111104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66001536"/>
+        <c:axId val="80111104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -801,7 +804,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66000000"/>
+        <c:crossAx val="80109568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -812,8 +815,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86773547094188475"/>
-          <c:y val="0.37152777777777846"/>
+          <c:x val="0.86773547094188486"/>
+          <c:y val="0.37152777777777857"/>
           <c:w val="0.11422845691382746"/>
           <c:h val="0.25"/>
         </c:manualLayout>
@@ -824,7 +827,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000004" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000004" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1154,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1911,10 +1914,10 @@
         <v>117</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D19">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E19" s="10">
         <v>70</v>
@@ -1924,11 +1927,11 @@
       </c>
       <c r="G19">
         <f>SUMIF('Horas insumidas'!$E$6:$E$135,A19,'Horas insumidas'!$F$6:$F$135)</f>
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>-23</v>
+        <v>-26</v>
       </c>
       <c r="I19">
         <f t="shared" si="1"/>
@@ -2021,11 +2024,11 @@
       </c>
       <c r="G24">
         <f>SUM(G2:G20)</f>
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="H24">
         <f>SUM(H2:H20)</f>
-        <v>-95</v>
+        <v>-98</v>
       </c>
       <c r="I24">
         <f>SUM(I2:I20)</f>
@@ -2045,8 +2048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+    <sheetView topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3528,6 +3531,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="99" spans="2:6">
+      <c r="B99" s="1">
+        <v>40478</v>
+      </c>
+      <c r="C99" t="s">
+        <v>33</v>
+      </c>
+      <c r="D99" t="s">
+        <v>130</v>
+      </c>
+      <c r="E99" t="s">
+        <v>112</v>
+      </c>
+      <c r="F99">
+        <v>3</v>
+      </c>
+    </row>
     <row r="110" spans="2:6">
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -3537,7 +3557,7 @@
       </c>
       <c r="F110" s="3">
         <f>SUM(F80:F109)</f>
-        <v>43.5</v>
+        <v>46.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
S-01021 - Se agrega el importe de la hora de la campaña según el nivel. Se agregan colores.
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Earned Value" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="133">
   <si>
     <t>Id</t>
   </si>
@@ -409,6 +409,12 @@
   </si>
   <si>
     <t>Métrica AUX_TM</t>
+  </si>
+  <si>
+    <t>duilio</t>
+  </si>
+  <si>
+    <t>Modificando pantalla de sueldo</t>
   </si>
 </sst>
 </file>
@@ -761,11 +767,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="80109568"/>
-        <c:axId val="80111104"/>
+        <c:axId val="80044032"/>
+        <c:axId val="80045568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80109568"/>
+        <c:axId val="80044032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -789,14 +795,14 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80111104"/>
+        <c:crossAx val="80045568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80111104"/>
+        <c:axId val="80045568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -804,7 +810,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80109568"/>
+        <c:crossAx val="80044032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -815,8 +821,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86773547094188486"/>
-          <c:y val="0.37152777777777857"/>
+          <c:x val="0.86773547094188508"/>
+          <c:y val="0.37152777777777868"/>
           <c:w val="0.11422845691382746"/>
           <c:h val="0.25"/>
         </c:manualLayout>
@@ -827,7 +833,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000422" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000422" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1157,7 +1163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -2048,8 +2054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F110"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3548,6 +3554,23 @@
         <v>3</v>
       </c>
     </row>
+    <row r="100" spans="2:6">
+      <c r="B100" s="1">
+        <v>40478</v>
+      </c>
+      <c r="C100" t="s">
+        <v>131</v>
+      </c>
+      <c r="D100" t="s">
+        <v>132</v>
+      </c>
+      <c r="E100" t="s">
+        <v>127</v>
+      </c>
+      <c r="F100">
+        <v>2</v>
+      </c>
+    </row>
     <row r="110" spans="2:6">
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -3557,7 +3580,7 @@
       </c>
       <c r="F110" s="3">
         <f>SUM(F80:F109)</f>
-        <v>46.5</v>
+        <v>48.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
S-01021 - Se agrega selección del período en la pantalla de sueldo.
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="134">
   <si>
     <t>Id</t>
   </si>
@@ -415,6 +415,9 @@
   </si>
   <si>
     <t>Modificando pantalla de sueldo</t>
+  </si>
+  <si>
+    <t>Agregando selección del período para el salario</t>
   </si>
 </sst>
 </file>
@@ -767,11 +770,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="80044032"/>
-        <c:axId val="80045568"/>
+        <c:axId val="79052800"/>
+        <c:axId val="79054336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80044032"/>
+        <c:axId val="79052800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -795,14 +798,14 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80045568"/>
+        <c:crossAx val="79054336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80045568"/>
+        <c:axId val="79054336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -810,7 +813,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80044032"/>
+        <c:crossAx val="79052800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -821,8 +824,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86773547094188508"/>
-          <c:y val="0.37152777777777868"/>
+          <c:x val="0.8677354709418853"/>
+          <c:y val="0.37152777777777879"/>
           <c:w val="0.11422845691382746"/>
           <c:h val="0.25"/>
         </c:manualLayout>
@@ -833,7 +836,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000422" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000422" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000433" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000433" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2055,7 +2058,7 @@
   <dimension ref="B1:F110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="F101" sqref="F101"/>
+      <selection activeCell="F102" sqref="F102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3571,6 +3574,23 @@
         <v>2</v>
       </c>
     </row>
+    <row r="101" spans="2:6">
+      <c r="B101" s="1">
+        <v>40478</v>
+      </c>
+      <c r="C101" t="s">
+        <v>33</v>
+      </c>
+      <c r="D101" t="s">
+        <v>133</v>
+      </c>
+      <c r="E101" t="s">
+        <v>127</v>
+      </c>
+      <c r="F101">
+        <v>3</v>
+      </c>
+    </row>
     <row r="110" spans="2:6">
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -3580,7 +3600,7 @@
       </c>
       <c r="F110" s="3">
         <f>SUM(F80:F109)</f>
-        <v>48.5</v>
+        <v>51.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TK-01038 - Correcciones en el sueldo de horas extra y en horas productivas
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Earned Value" sheetId="1" r:id="rId1"/>
     <sheet name="Horas insumidas" sheetId="2" r:id="rId2"/>
     <sheet name="Estadísticas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="135">
   <si>
     <t>Id</t>
   </si>
@@ -418,13 +418,16 @@
   </si>
   <si>
     <t>Agregando selección del período para el salario</t>
+  </si>
+  <si>
+    <t>Sueldo Hs extra y Horas productivas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -574,13 +577,29 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="es-AR"/>
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -595,6 +614,7 @@
       </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -656,6 +676,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -712,6 +733,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -768,18 +790,31 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="79052800"/>
-        <c:axId val="79054336"/>
+        <c:smooth val="0"/>
+        <c:axId val="128589824"/>
+        <c:axId val="97620480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="79052800"/>
+        <c:axId val="128589824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr rot="0" vert="horz"/>
@@ -795,25 +830,29 @@
                 <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79054336"/>
+        <c:crossAx val="97620480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79054336"/>
+        <c:axId val="97620480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79052800"/>
+        <c:crossAx val="128589824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -830,9 +869,11 @@
           <c:h val="0.25"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -954,6 +995,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -988,6 +1030,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1163,14 +1206,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="51.85546875" customWidth="1"/>
@@ -1183,7 +1226,7 @@
     <col min="9" max="9" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1218,7 +1261,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
@@ -1259,7 +1302,7 @@
         <v>1.1940298507462686</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
@@ -1300,7 +1343,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
@@ -1341,7 +1384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
@@ -1382,7 +1425,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>18</v>
       </c>
@@ -1423,7 +1466,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>20</v>
       </c>
@@ -1464,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>22</v>
       </c>
@@ -1505,7 +1548,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>24</v>
       </c>
@@ -1546,7 +1589,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>26</v>
       </c>
@@ -1587,7 +1630,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>81</v>
       </c>
@@ -1628,7 +1671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>83</v>
       </c>
@@ -1669,7 +1712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>85</v>
       </c>
@@ -1710,7 +1753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>87</v>
       </c>
@@ -1751,7 +1794,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>75</v>
       </c>
@@ -1792,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>90</v>
       </c>
@@ -1833,7 +1876,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>92</v>
       </c>
@@ -1874,7 +1917,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>71</v>
       </c>
@@ -1915,7 +1958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>112</v>
       </c>
@@ -1932,30 +1975,30 @@
         <v>70</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="G19">
         <f>SUMIF('Horas insumidas'!$E$6:$E$135,A19,'Horas insumidas'!$F$6:$F$135)</f>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>-26</v>
+        <v>40</v>
       </c>
       <c r="I19">
         <f t="shared" si="1"/>
-        <v>-70</v>
+        <v>0</v>
       </c>
       <c r="J19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>2.3333333333333335</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>119</v>
       </c>
@@ -1963,16 +2006,16 @@
         <v>118</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D20">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E20" s="10">
         <v>10</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G20">
         <f>SUMIF('Horas insumidas'!$E$6:$E$135,A20,'Horas insumidas'!$F$6:$F$135)</f>
@@ -1980,22 +2023,22 @@
       </c>
       <c r="H20">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>8</v>
       </c>
       <c r="I20">
         <f t="shared" si="1"/>
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="J20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -2003,7 +2046,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>102</v>
       </c>
@@ -2011,7 +2054,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>121</v>
       </c>
@@ -2019,7 +2062,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>28</v>
       </c>
@@ -2029,22 +2072,22 @@
       </c>
       <c r="F24">
         <f>SUM(F2:F20)</f>
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="G24">
         <f>SUM(G2:G20)</f>
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="H24">
         <f>SUM(H2:H20)</f>
-        <v>-98</v>
+        <v>-22</v>
       </c>
       <c r="I24">
         <f>SUM(I2:I20)</f>
-        <v>-493</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>-413</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
     </row>
   </sheetData>
@@ -2054,14 +2097,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="F102" sqref="F102"/>
+    <sheetView topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="F103" sqref="F103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
@@ -2070,8 +2113,8 @@
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>29</v>
       </c>
@@ -2088,7 +2131,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:6">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>40428</v>
       </c>
@@ -2102,7 +2145,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>40429</v>
       </c>
@@ -2116,7 +2159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>40429</v>
       </c>
@@ -2130,7 +2173,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>40431</v>
       </c>
@@ -2144,7 +2187,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>40432</v>
       </c>
@@ -2158,7 +2201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>40432</v>
       </c>
@@ -2172,7 +2215,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>40432</v>
       </c>
@@ -2186,7 +2229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>40432</v>
       </c>
@@ -2200,7 +2243,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>40433</v>
       </c>
@@ -2214,7 +2257,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
         <v>46</v>
       </c>
@@ -2223,7 +2266,7 @@
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>40435</v>
       </c>
@@ -2240,7 +2283,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>40435</v>
       </c>
@@ -2257,7 +2300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>40435</v>
       </c>
@@ -2274,7 +2317,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>40435</v>
       </c>
@@ -2291,7 +2334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>40435</v>
       </c>
@@ -2308,7 +2351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>40435</v>
       </c>
@@ -2325,7 +2368,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>40436</v>
       </c>
@@ -2342,7 +2385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>40436</v>
       </c>
@@ -2359,7 +2402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>40436</v>
       </c>
@@ -2376,7 +2419,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>40437</v>
       </c>
@@ -2393,7 +2436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>40438</v>
       </c>
@@ -2410,7 +2453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>40439</v>
       </c>
@@ -2427,7 +2470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>40439</v>
       </c>
@@ -2444,7 +2487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>40439</v>
       </c>
@@ -2461,7 +2504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>40441</v>
       </c>
@@ -2478,7 +2521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>40442</v>
       </c>
@@ -2495,7 +2538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>40442</v>
       </c>
@@ -2512,7 +2555,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>40442</v>
       </c>
@@ -2529,7 +2572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:6">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>40442</v>
       </c>
@@ -2546,7 +2589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
         <v>40444</v>
       </c>
@@ -2563,7 +2606,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="2:6">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
         <v>40444</v>
       </c>
@@ -2580,7 +2623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:6">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <v>40444</v>
       </c>
@@ -2597,7 +2640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:6">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <v>40444</v>
       </c>
@@ -2614,7 +2657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="2:6">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <v>40445</v>
       </c>
@@ -2631,7 +2674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>40445</v>
       </c>
@@ -2648,7 +2691,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="38" spans="2:6">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
         <v>40445</v>
       </c>
@@ -2665,7 +2708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:6">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>40445</v>
       </c>
@@ -2682,7 +2725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="2:6">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
         <v>40446</v>
       </c>
@@ -2699,7 +2742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
         <v>40448</v>
       </c>
@@ -2716,7 +2759,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="42" spans="2:6">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -2728,7 +2771,7 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="43" spans="2:6">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="12" t="s">
         <v>61</v>
       </c>
@@ -2737,7 +2780,7 @@
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
     </row>
-    <row r="44" spans="2:6">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="1">
         <v>40450</v>
       </c>
@@ -2754,7 +2797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="2:6">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" s="1">
         <v>40450</v>
       </c>
@@ -2771,7 +2814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:6">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="1">
         <v>40450</v>
       </c>
@@ -2788,7 +2831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:6">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="1">
         <v>40451</v>
       </c>
@@ -2805,7 +2848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:6">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="1">
         <v>40452</v>
       </c>
@@ -2822,7 +2865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:6">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
         <v>40453</v>
       </c>
@@ -2839,7 +2882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="30">
+    <row r="50" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B50" s="1">
         <v>40452</v>
       </c>
@@ -2856,7 +2899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="2:6" ht="60">
+    <row r="51" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B51" s="1">
         <v>40453</v>
       </c>
@@ -2873,7 +2916,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="2:6" ht="18" customHeight="1">
+    <row r="52" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="1">
         <v>40454</v>
       </c>
@@ -2890,7 +2933,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="53" spans="2:6">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="1">
         <v>40454</v>
       </c>
@@ -2907,7 +2950,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="54" spans="2:6">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="1">
         <v>40454</v>
       </c>
@@ -2924,7 +2967,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="55" spans="2:6">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="1">
         <v>40454</v>
       </c>
@@ -2941,7 +2984,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="2:6">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="1">
         <v>40455</v>
       </c>
@@ -2958,7 +3001,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="57" spans="2:6">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="1">
         <v>40455</v>
       </c>
@@ -2975,7 +3018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="2:6">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="1">
         <v>40456</v>
       </c>
@@ -2992,7 +3035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:6">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="1">
         <v>40456</v>
       </c>
@@ -3009,7 +3052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="2:6">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="1">
         <v>40457</v>
       </c>
@@ -3026,7 +3069,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="2:6">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="1">
         <v>40458</v>
       </c>
@@ -3043,7 +3086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="2:6">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="1">
         <v>40459</v>
       </c>
@@ -3060,7 +3103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="2:6">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63" s="1">
         <v>40460</v>
       </c>
@@ -3077,7 +3120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="2:6">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="1">
         <v>40462</v>
       </c>
@@ -3094,7 +3137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="2:6">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="1">
         <v>40463</v>
       </c>
@@ -3111,7 +3154,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="2:6">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="1">
         <v>40464</v>
       </c>
@@ -3128,7 +3171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="2:6">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="1">
         <v>40465</v>
       </c>
@@ -3145,7 +3188,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="68" spans="2:6">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" s="1">
         <v>40465</v>
       </c>
@@ -3162,7 +3205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="2:6">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69" s="1">
         <v>40465</v>
       </c>
@@ -3179,7 +3222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="2:6">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="1">
         <v>40465</v>
       </c>
@@ -3196,7 +3239,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="2:6">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="1">
         <v>40466</v>
       </c>
@@ -3213,7 +3256,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="2:6">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72" s="1">
         <v>40467</v>
       </c>
@@ -3230,7 +3273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:6">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
@@ -3242,7 +3285,7 @@
         <v>66.5</v>
       </c>
     </row>
-    <row r="81" spans="2:6">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81" s="12" t="s">
         <v>62</v>
       </c>
@@ -3251,7 +3294,7 @@
       <c r="E81" s="12"/>
       <c r="F81" s="12"/>
     </row>
-    <row r="82" spans="2:6">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" s="1">
         <v>40471</v>
       </c>
@@ -3268,7 +3311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="2:6">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B83" s="1">
         <v>40471</v>
       </c>
@@ -3285,7 +3328,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="84" spans="2:6">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B84" s="1">
         <v>40472</v>
       </c>
@@ -3302,7 +3345,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="2:6">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85" s="1">
         <v>40472</v>
       </c>
@@ -3319,7 +3362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="2:6">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B86" s="1">
         <v>40472</v>
       </c>
@@ -3336,7 +3379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="2:6">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87" s="1">
         <v>40472</v>
       </c>
@@ -3353,7 +3396,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="2:6">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B88" s="1">
         <v>40473</v>
       </c>
@@ -3370,7 +3413,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="89" spans="2:6">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B89" s="1">
         <v>40474</v>
       </c>
@@ -3387,7 +3430,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="90" spans="2:6">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B90" s="1">
         <v>40474</v>
       </c>
@@ -3404,7 +3447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="2:6">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B91" s="1">
         <v>40474</v>
       </c>
@@ -3421,7 +3464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="2:6">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B92" s="1">
         <v>40474</v>
       </c>
@@ -3438,7 +3481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="2:6">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B93" s="1">
         <v>40474</v>
       </c>
@@ -3455,7 +3498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="2:6">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B94" s="1">
         <v>40475</v>
       </c>
@@ -3472,7 +3515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="2:6">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B95" s="1">
         <v>40475</v>
       </c>
@@ -3489,7 +3532,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="2:6">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B96" s="1">
         <v>40475</v>
       </c>
@@ -3506,7 +3549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="2:6">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B97" s="1">
         <v>40475</v>
       </c>
@@ -3523,7 +3566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="2:6">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B98" s="1">
         <v>40476</v>
       </c>
@@ -3540,7 +3583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:6">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B99" s="1">
         <v>40478</v>
       </c>
@@ -3557,7 +3600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="2:6">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B100" s="1">
         <v>40478</v>
       </c>
@@ -3574,7 +3617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="2:6">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B101" s="1">
         <v>40478</v>
       </c>
@@ -3591,7 +3634,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="2:6">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B102" s="1">
+        <v>40478</v>
+      </c>
+      <c r="C102" t="s">
+        <v>65</v>
+      </c>
+      <c r="D102" t="s">
+        <v>134</v>
+      </c>
+      <c r="E102" t="s">
+        <v>112</v>
+      </c>
+      <c r="F102">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
@@ -3600,7 +3660,7 @@
       </c>
       <c r="F110" s="3">
         <f>SUM(F80:F109)</f>
-        <v>51.5</v>
+        <v>55.5</v>
       </c>
     </row>
   </sheetData>
@@ -3616,20 +3676,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B19:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="19" spans="2:9">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>3</v>
       </c>
@@ -3652,7 +3712,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>46</v>
       </c>
@@ -3685,7 +3745,7 @@
         <v>1.1940298507462686</v>
       </c>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>61</v>
       </c>
@@ -3715,7 +3775,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>62</v>
       </c>
@@ -3745,7 +3805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>63</v>
       </c>
@@ -3770,7 +3830,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
S-01020 - Saco librerias innecesarias
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="137">
   <si>
     <t>Id</t>
   </si>
@@ -424,6 +424,9 @@
   </si>
   <si>
     <t>Analisis Cuadrados minimos</t>
+  </si>
+  <si>
+    <t>Gráfica de Cuadrados minimos</t>
   </si>
 </sst>
 </file>
@@ -780,13 +783,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="62313984"/>
-        <c:axId val="62315520"/>
+        <c:axId val="62899712"/>
+        <c:axId val="62901248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="62313984"/>
+        <c:axId val="62899712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -810,14 +812,14 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62315520"/>
+        <c:crossAx val="62901248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62315520"/>
+        <c:axId val="62901248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -825,7 +827,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62313984"/>
+        <c:crossAx val="62899712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -836,8 +838,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86773547094188552"/>
-          <c:y val="0.37152777777777896"/>
+          <c:x val="0.86773547094188574"/>
+          <c:y val="0.37152777777777907"/>
           <c:w val="0.11422845691382746"/>
           <c:h val="0.25"/>
         </c:manualLayout>
@@ -848,7 +850,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000444" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000444" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000455" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000455" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1948,11 +1950,11 @@
       </c>
       <c r="G19">
         <f>SUMIF('Horas insumidas'!$E$6:$E$135,A19,'Horas insumidas'!$F$6:$F$135)</f>
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="I19">
         <f t="shared" si="1"/>
@@ -1964,7 +1966,7 @@
       </c>
       <c r="K19">
         <f t="shared" si="3"/>
-        <v>1.9444444444444444</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -2045,11 +2047,11 @@
       </c>
       <c r="G24">
         <f>SUM(G2:G20)</f>
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H24">
         <f>SUM(H2:H20)</f>
-        <v>-28</v>
+        <v>-32</v>
       </c>
       <c r="I24">
         <f>SUM(I2:I20)</f>
@@ -2069,15 +2071,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2851,7 +2853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="30">
+    <row r="50" spans="2:6" ht="17.25" customHeight="1">
       <c r="B50" s="1">
         <v>40452</v>
       </c>
@@ -2868,7 +2870,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="2:6" ht="60">
+    <row r="51" spans="2:6" ht="30">
       <c r="B51" s="1">
         <v>40453</v>
       </c>
@@ -3637,6 +3639,23 @@
         <v>6</v>
       </c>
     </row>
+    <row r="104" spans="2:6">
+      <c r="B104" s="1">
+        <v>40482</v>
+      </c>
+      <c r="C104" t="s">
+        <v>47</v>
+      </c>
+      <c r="D104" t="s">
+        <v>136</v>
+      </c>
+      <c r="E104" t="s">
+        <v>112</v>
+      </c>
+      <c r="F104">
+        <v>4</v>
+      </c>
+    </row>
     <row r="110" spans="2:6">
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -3646,7 +3665,7 @@
       </c>
       <c r="F110" s="3">
         <f>SUM(F80:F109)</f>
-        <v>61.5</v>
+        <v>65.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
S-01023 - horas duilio
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Earned Value" sheetId="1" r:id="rId1"/>
     <sheet name="Horas insumidas" sheetId="2" r:id="rId2"/>
     <sheet name="Estadísticas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="114210"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="143">
   <si>
     <t>Id</t>
   </si>
@@ -436,6 +436,15 @@
   </si>
   <si>
     <t>Calculo de metricas</t>
+  </si>
+  <si>
+    <t>Corrección sueldo variable</t>
+  </si>
+  <si>
+    <t>S-01023</t>
+  </si>
+  <si>
+    <t>Corrección de gráficos, mostrar todos los gráficos en la pantalla</t>
   </si>
 </sst>
 </file>
@@ -612,7 +621,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="es-AR"/>
   <c:chart>
     <c:plotArea>
       <c:layout>
@@ -620,10 +629,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.0140280561122245E-2"/>
+          <c:x val="7.0140280561122259E-2"/>
           <c:y val="4.8611111111111112E-2"/>
           <c:w val="0.70340681362725455"/>
-          <c:h val="0.82986111111111116"/>
+          <c:h val="0.82986111111111127"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -803,11 +812,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="39676160"/>
-        <c:axId val="39690624"/>
+        <c:axId val="66000384"/>
+        <c:axId val="66002304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39676160"/>
+        <c:axId val="66000384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -828,17 +837,17 @@
                 <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39690624"/>
+        <c:crossAx val="66002304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39690624"/>
+        <c:axId val="66002304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -846,7 +855,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39676160"/>
+        <c:crossAx val="66000384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -857,12 +866,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:wMode val="edge"/>
-          <c:hMode val="edge"/>
-          <c:x val="0.86773547094188375"/>
-          <c:y val="0.37152777777777779"/>
-          <c:w val="0.9819639278557114"/>
-          <c:h val="0.62152777777777779"/>
+          <c:x val="0.86773547094188386"/>
+          <c:y val="0.37152777777777796"/>
+          <c:w val="0.11422845691382744"/>
+          <c:h val="0.24999999999999983"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -871,7 +878,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000488" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000488" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -915,7 +922,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1274,7 +1281,7 @@
         <v>40</v>
       </c>
       <c r="G2">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A2,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A2,'Horas insumidas'!$F$6:$F$135)</f>
         <v>33.5</v>
       </c>
       <c r="H2">
@@ -1315,7 +1322,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A3,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A3,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H3">
@@ -1356,7 +1363,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A4,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A4,'Horas insumidas'!$F$6:$F$135)</f>
         <v>17</v>
       </c>
       <c r="H4">
@@ -1397,7 +1404,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A5,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A5,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H5">
@@ -1438,7 +1445,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A6,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A6,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H6">
@@ -1479,7 +1486,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A7,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A7,'Horas insumidas'!$F$6:$F$135)</f>
         <v>21</v>
       </c>
       <c r="H7">
@@ -1520,7 +1527,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A8,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A8,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H8">
@@ -1561,7 +1568,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A9,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A9,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H9">
@@ -1602,7 +1609,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A10,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A10,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H10">
@@ -1643,7 +1650,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A11,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A11,'Horas insumidas'!$F$6:$F$135)</f>
         <v>3.5</v>
       </c>
       <c r="H11">
@@ -1684,7 +1691,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A12,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A12,'Horas insumidas'!$F$6:$F$135)</f>
         <v>5</v>
       </c>
       <c r="H12">
@@ -1725,7 +1732,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A13,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A13,'Horas insumidas'!$F$6:$F$135)</f>
         <v>4.5</v>
       </c>
       <c r="H13">
@@ -1766,7 +1773,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A14,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A14,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H14">
@@ -1807,7 +1814,7 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A15,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A15,'Horas insumidas'!$F$6:$F$135)</f>
         <v>8</v>
       </c>
       <c r="H15">
@@ -1848,7 +1855,7 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A16,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A16,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H16">
@@ -1889,7 +1896,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A17,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A17,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H17">
@@ -1930,7 +1937,7 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A18,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A18,'Horas insumidas'!$F$6:$F$135)</f>
         <v>17.5</v>
       </c>
       <c r="H18">
@@ -1970,7 +1977,7 @@
         <v>70</v>
       </c>
       <c r="G19">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A19,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A19,'Horas insumidas'!$F$6:$F$135)</f>
         <v>44.5</v>
       </c>
       <c r="H19">
@@ -2010,7 +2017,7 @@
         <v>10</v>
       </c>
       <c r="G20">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A20,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A20,'Horas insumidas'!$F$6:$F$135)</f>
         <v>2</v>
       </c>
       <c r="H20">
@@ -2090,10 +2097,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F110"/>
+  <dimension ref="B1:F115"/>
   <sheetViews>
-    <sheetView topLeftCell="B84" workbookViewId="0">
-      <selection activeCell="F109" sqref="F109"/>
+    <sheetView tabSelected="1" topLeftCell="B99" workbookViewId="0">
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3757,11 +3764,55 @@
         <v>72</v>
       </c>
     </row>
+    <row r="113" spans="2:6">
+      <c r="B113" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C113" s="12"/>
+      <c r="D113" s="12"/>
+      <c r="E113" s="12"/>
+      <c r="F113" s="12"/>
+    </row>
+    <row r="114" spans="2:6">
+      <c r="B114" s="1">
+        <v>40485</v>
+      </c>
+      <c r="C114" t="s">
+        <v>33</v>
+      </c>
+      <c r="D114" t="s">
+        <v>140</v>
+      </c>
+      <c r="E114" t="s">
+        <v>141</v>
+      </c>
+      <c r="F114">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6">
+      <c r="B115" s="1">
+        <v>40486</v>
+      </c>
+      <c r="C115" t="s">
+        <v>33</v>
+      </c>
+      <c r="D115" t="s">
+        <v>142</v>
+      </c>
+      <c r="E115" t="s">
+        <v>141</v>
+      </c>
+      <c r="F115">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B43:F43"/>
     <mergeCell ref="B81:F81"/>
+    <mergeCell ref="B113:F113"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3773,7 +3824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B19:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -3812,15 +3863,15 @@
         <v>46</v>
       </c>
       <c r="C20" s="11">
-        <f ca="1">'Earned Value'!E2</f>
+        <f>'Earned Value'!E2</f>
         <v>40</v>
       </c>
       <c r="D20" s="11">
-        <f ca="1">'Earned Value'!F2</f>
+        <f>'Earned Value'!F2</f>
         <v>40</v>
       </c>
       <c r="E20" s="11">
-        <f ca="1">'Earned Value'!G2</f>
+        <f>'Earned Value'!G2</f>
         <v>33.5</v>
       </c>
       <c r="F20" s="11">

</xml_diff>

<commit_message>
reporte de avance 20101108
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Earned Value" sheetId="1" r:id="rId1"/>
     <sheet name="Horas insumidas" sheetId="2" r:id="rId2"/>
     <sheet name="Estadísticas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="148">
   <si>
     <t>Id</t>
   </si>
@@ -445,6 +445,21 @@
   </si>
   <si>
     <t>Corrección de gráficos, mostrar todos los gráficos en la pantalla</t>
+  </si>
+  <si>
+    <t>Parseo STS</t>
+  </si>
+  <si>
+    <t>Metrica NCH</t>
+  </si>
+  <si>
+    <t>Metrica PCT</t>
+  </si>
+  <si>
+    <t>T-01005</t>
+  </si>
+  <si>
+    <t>Total Sprint 4</t>
   </si>
 </sst>
 </file>
@@ -621,7 +636,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="es-AR"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:plotArea>
       <c:layout>
@@ -629,10 +644,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.0140280561122259E-2"/>
+          <c:x val="7.0140280561122245E-2"/>
           <c:y val="4.8611111111111112E-2"/>
           <c:w val="0.70340681362725455"/>
-          <c:h val="0.82986111111111127"/>
+          <c:h val="0.82986111111111116"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -690,10 +705,10 @@
                   <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>213</c:v>
+                  <c:v>233</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>253</c:v>
+                  <c:v>273</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -751,6 +766,9 @@
                 <c:pt idx="2">
                   <c:v>153</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>190</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -807,16 +825,19 @@
                 <c:pt idx="2">
                   <c:v>163</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>185</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="66000384"/>
-        <c:axId val="66002304"/>
+        <c:axId val="39676160"/>
+        <c:axId val="39690624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66000384"/>
+        <c:axId val="39676160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -837,17 +858,17 @@
                 <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66002304"/>
+        <c:crossAx val="39690624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66002304"/>
+        <c:axId val="39690624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,7 +876,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66000384"/>
+        <c:crossAx val="39676160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -866,10 +887,12 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86773547094188386"/>
-          <c:y val="0.37152777777777796"/>
-          <c:w val="0.11422845691382744"/>
-          <c:h val="0.24999999999999983"/>
+          <c:wMode val="edge"/>
+          <c:hMode val="edge"/>
+          <c:x val="0.86773547094188375"/>
+          <c:y val="0.37152777777777779"/>
+          <c:w val="0.9819639278557114"/>
+          <c:h val="0.62152777777777779"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -878,7 +901,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000488" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000488" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -901,7 +924,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1025" name="Chart 1"/>
+        <xdr:cNvPr id="2049" name="Chart 1"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -922,7 +945,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1281,7 +1304,7 @@
         <v>40</v>
       </c>
       <c r="G2">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A2,'Horas insumidas'!$F$6:$F$135)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A2,'Horas insumidas'!$F$6:$F$135)</f>
         <v>33.5</v>
       </c>
       <c r="H2">
@@ -1322,7 +1345,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A3,'Horas insumidas'!$F$6:$F$135)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A3,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H3">
@@ -1363,12 +1386,12 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A4,'Horas insumidas'!$F$6:$F$135)</f>
-        <v>17</v>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A4,'Horas insumidas'!$F$6:$F$135)</f>
+        <v>20.5</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H20" si="0">F4-G4</f>
-        <v>-17</v>
+        <v>-20.5</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I20" si="1">F4-E4</f>
@@ -1404,7 +1427,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A5,'Horas insumidas'!$F$6:$F$135)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A5,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H5">
@@ -1445,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A6,'Horas insumidas'!$F$6:$F$135)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A6,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H6">
@@ -1486,7 +1509,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A7,'Horas insumidas'!$F$6:$F$135)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A7,'Horas insumidas'!$F$6:$F$135)</f>
         <v>21</v>
       </c>
       <c r="H7">
@@ -1527,7 +1550,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A8,'Horas insumidas'!$F$6:$F$135)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A8,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H8">
@@ -1568,7 +1591,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A9,'Horas insumidas'!$F$6:$F$135)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A9,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H9">
@@ -1609,7 +1632,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A10,'Horas insumidas'!$F$6:$F$135)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A10,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H10">
@@ -1650,7 +1673,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A11,'Horas insumidas'!$F$6:$F$135)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A11,'Horas insumidas'!$F$6:$F$135)</f>
         <v>3.5</v>
       </c>
       <c r="H11">
@@ -1691,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A12,'Horas insumidas'!$F$6:$F$135)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A12,'Horas insumidas'!$F$6:$F$135)</f>
         <v>5</v>
       </c>
       <c r="H12">
@@ -1732,7 +1755,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A13,'Horas insumidas'!$F$6:$F$135)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A13,'Horas insumidas'!$F$6:$F$135)</f>
         <v>4.5</v>
       </c>
       <c r="H13">
@@ -1773,12 +1796,12 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A14,'Horas insumidas'!$F$6:$F$135)</f>
-        <v>0</v>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A14,'Horas insumidas'!$F$6:$F$135)</f>
+        <v>2</v>
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="I14">
         <f t="shared" si="1"/>
@@ -1788,9 +1811,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K14" t="e">
+      <c r="K14">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1814,7 +1837,7 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A15,'Horas insumidas'!$F$6:$F$135)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A15,'Horas insumidas'!$F$6:$F$135)</f>
         <v>8</v>
       </c>
       <c r="H15">
@@ -1855,7 +1878,7 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A16,'Horas insumidas'!$F$6:$F$135)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A16,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H16">
@@ -1896,7 +1919,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A17,'Horas insumidas'!$F$6:$F$135)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A17,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H17">
@@ -1937,7 +1960,7 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A18,'Horas insumidas'!$F$6:$F$135)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A18,'Horas insumidas'!$F$6:$F$135)</f>
         <v>17.5</v>
       </c>
       <c r="H18">
@@ -1977,7 +2000,7 @@
         <v>70</v>
       </c>
       <c r="G19">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A19,'Horas insumidas'!$F$6:$F$135)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A19,'Horas insumidas'!$F$6:$F$135)</f>
         <v>44.5</v>
       </c>
       <c r="H19">
@@ -2017,7 +2040,7 @@
         <v>10</v>
       </c>
       <c r="G20">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A20,'Horas insumidas'!$F$6:$F$135)</f>
+        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A20,'Horas insumidas'!$F$6:$F$135)</f>
         <v>2</v>
       </c>
       <c r="H20">
@@ -2075,11 +2098,11 @@
       </c>
       <c r="G24">
         <f>SUM(G2:G20)</f>
-        <v>156.5</v>
+        <v>162</v>
       </c>
       <c r="H24">
         <f>SUM(H2:H20)</f>
-        <v>-36.5</v>
+        <v>-42</v>
       </c>
       <c r="I24">
         <f>SUM(I2:I20)</f>
@@ -2097,10 +2120,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F115"/>
+  <dimension ref="B1:F137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B99" workbookViewId="0">
-      <selection activeCell="D115" sqref="D115"/>
+    <sheetView topLeftCell="B111" workbookViewId="0">
+      <selection activeCell="F138" sqref="F138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3805,6 +3828,103 @@
       </c>
       <c r="F115">
         <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="2:6">
+      <c r="B116" s="1">
+        <v>40484</v>
+      </c>
+      <c r="C116" t="s">
+        <v>95</v>
+      </c>
+      <c r="D116" t="s">
+        <v>143</v>
+      </c>
+      <c r="E116" t="s">
+        <v>87</v>
+      </c>
+      <c r="F116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="2:6">
+      <c r="B117" s="1">
+        <v>40484</v>
+      </c>
+      <c r="C117" t="s">
+        <v>95</v>
+      </c>
+      <c r="D117" t="s">
+        <v>144</v>
+      </c>
+      <c r="E117" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="2:6">
+      <c r="B118" s="1">
+        <v>40485</v>
+      </c>
+      <c r="C118" t="s">
+        <v>95</v>
+      </c>
+      <c r="D118" t="s">
+        <v>145</v>
+      </c>
+      <c r="E118" t="s">
+        <v>14</v>
+      </c>
+      <c r="F118">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="119" spans="2:6">
+      <c r="B119" s="1">
+        <v>40485</v>
+      </c>
+      <c r="C119" t="s">
+        <v>95</v>
+      </c>
+      <c r="D119" t="s">
+        <v>55</v>
+      </c>
+      <c r="E119" t="s">
+        <v>146</v>
+      </c>
+      <c r="F119">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="120" spans="2:6">
+      <c r="B120" s="1">
+        <v>40489</v>
+      </c>
+      <c r="C120" t="s">
+        <v>95</v>
+      </c>
+      <c r="D120" t="s">
+        <v>53</v>
+      </c>
+      <c r="E120" t="s">
+        <v>146</v>
+      </c>
+      <c r="F120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="2:6">
+      <c r="B137" s="3"/>
+      <c r="C137" s="3"/>
+      <c r="D137" s="3"/>
+      <c r="E137" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F137" s="3">
+        <f>SUM(F114:F136)</f>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -3824,8 +3944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B19:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3863,15 +3983,15 @@
         <v>46</v>
       </c>
       <c r="C20" s="11">
-        <f>'Earned Value'!E2</f>
+        <f ca="1">'Earned Value'!E2</f>
         <v>40</v>
       </c>
       <c r="D20" s="11">
-        <f>'Earned Value'!F2</f>
+        <f ca="1">'Earned Value'!F2</f>
         <v>40</v>
       </c>
       <c r="E20" s="11">
-        <f>'Earned Value'!G2</f>
+        <f ca="1">'Earned Value'!G2</f>
         <v>33.5</v>
       </c>
       <c r="F20" s="11">
@@ -3956,26 +4076,29 @@
         <v>63</v>
       </c>
       <c r="C23" s="11">
-        <f>C22+40</f>
-        <v>213</v>
-      </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
+        <v>233</v>
+      </c>
+      <c r="D23" s="11">
+        <v>190</v>
+      </c>
+      <c r="E23" s="11">
+        <v>185</v>
+      </c>
       <c r="F23" s="11">
         <f>D23-E23</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G23" s="11">
         <f>D23-C23</f>
-        <v>-213</v>
+        <v>-43</v>
       </c>
       <c r="H23" s="11">
         <f>D23/C23</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="11" t="e">
+        <v>0.81545064377682408</v>
+      </c>
+      <c r="I23" s="11">
         <f>D23/E23</f>
-        <v>#DIV/0!</v>
+        <v>1.027027027027027</v>
       </c>
     </row>
     <row r="24" spans="2:9">
@@ -3984,7 +4107,7 @@
       </c>
       <c r="C24" s="11">
         <f>C23+40</f>
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
@@ -3994,7 +4117,7 @@
       </c>
       <c r="G24" s="11">
         <f>D24-C24</f>
-        <v>-253</v>
+        <v>-273</v>
       </c>
       <c r="H24" s="11">
         <f>D24/C24</f>

</xml_diff>

<commit_message>
TK-01046 - Se quitó el valor no satisfactorio de la campaña y se harcodeó siempre en cero.
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Horas insumidas" sheetId="2" r:id="rId2"/>
     <sheet name="Estadísticas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="114210"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="153">
   <si>
     <t>Id</t>
   </si>
@@ -460,6 +460,21 @@
   </si>
   <si>
     <t>Total Sprint 4</t>
+  </si>
+  <si>
+    <t>Agregados sueldo hs extra</t>
+  </si>
+  <si>
+    <t>Tareas de administracion para el cuarto Sprint</t>
+  </si>
+  <si>
+    <t>Correcciones sprint 3</t>
+  </si>
+  <si>
+    <t>S01024</t>
+  </si>
+  <si>
+    <t>Métricas para agentes: 3 métricas</t>
   </si>
 </sst>
 </file>
@@ -636,7 +651,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="es-AR"/>
   <c:chart>
     <c:plotArea>
       <c:layout>
@@ -644,10 +659,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.0140280561122245E-2"/>
+          <c:x val="7.0140280561122259E-2"/>
           <c:y val="4.8611111111111112E-2"/>
           <c:w val="0.70340681362725455"/>
-          <c:h val="0.82986111111111116"/>
+          <c:h val="0.82986111111111138"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -705,10 +720,10 @@
                   <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>233</c:v>
+                  <c:v>285</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>273</c:v>
+                  <c:v>325</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -767,7 +782,7 @@
                   <c:v>153</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>190</c:v>
+                  <c:v>216</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -826,18 +841,18 @@
                   <c:v>163</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>185</c:v>
+                  <c:v>195</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="39676160"/>
-        <c:axId val="39690624"/>
+        <c:axId val="67049728"/>
+        <c:axId val="67072000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39676160"/>
+        <c:axId val="67049728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -858,17 +873,17 @@
                 <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39690624"/>
+        <c:crossAx val="67072000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39690624"/>
+        <c:axId val="67072000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,7 +891,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39676160"/>
+        <c:crossAx val="67049728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -887,12 +902,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:wMode val="edge"/>
-          <c:hMode val="edge"/>
-          <c:x val="0.86773547094188375"/>
-          <c:y val="0.37152777777777779"/>
-          <c:w val="0.9819639278557114"/>
-          <c:h val="0.62152777777777779"/>
+          <c:x val="0.86773547094188408"/>
+          <c:y val="0.37152777777777807"/>
+          <c:w val="0.11422845691382745"/>
+          <c:h val="0.24999999999999989"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -901,7 +914,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000522" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000522" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -945,7 +958,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1229,23 +1242,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="51.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1304,7 +1317,7 @@
         <v>40</v>
       </c>
       <c r="G2">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A2,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A2,'Horas insumidas'!$F$6:$F$135)</f>
         <v>33.5</v>
       </c>
       <c r="H2">
@@ -1338,14 +1351,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="10">
-        <f>40</f>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A3,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A3,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H3">
@@ -1354,7 +1366,7 @@
       </c>
       <c r="I3">
         <f>F3-E3</f>
-        <v>-40</v>
+        <v>-20</v>
       </c>
       <c r="J3">
         <f>F3/E3</f>
@@ -1373,37 +1385,37 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E4" s="10">
         <f>40</f>
         <v>40</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G4">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A4,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A4,'Horas insumidas'!$F$6:$F$135)</f>
         <v>20.5</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H20" si="0">F4-G4</f>
-        <v>-20.5</v>
+        <f t="shared" ref="H4:H19" si="0">F4-G4</f>
+        <v>19.5</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I20" si="1">F4-E4</f>
-        <v>-40</v>
+        <f t="shared" ref="I4:I19" si="1">F4-E4</f>
+        <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J20" si="2">F4/E4</f>
-        <v>0</v>
+        <f t="shared" ref="J4:J19" si="2">F4/E4</f>
+        <v>1</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K20" si="3">F4/G4</f>
-        <v>0</v>
+        <f t="shared" ref="K4:K19" si="3">F4/G4</f>
+        <v>1.9512195121951219</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1420,14 +1432,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="10">
-        <f>40</f>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A5,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A5,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H5">
@@ -1436,7 +1447,7 @@
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>-40</v>
+        <v>-20</v>
       </c>
       <c r="J5">
         <f t="shared" si="2"/>
@@ -1461,14 +1472,13 @@
         <v>0</v>
       </c>
       <c r="E6" s="10">
-        <f>40</f>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A6,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A6,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H6">
@@ -1477,7 +1487,7 @@
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>-40</v>
+        <v>-20</v>
       </c>
       <c r="J6">
         <f t="shared" si="2"/>
@@ -1496,37 +1506,37 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E7" s="10">
         <f>20</f>
         <v>20</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G7">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A7,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A7,'Horas insumidas'!$F$6:$F$135)</f>
         <v>21</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>-21</v>
+        <v>-1</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.95238095238095233</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1550,7 +1560,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A8,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A8,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H8">
@@ -1591,7 +1601,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A9,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A9,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H9">
@@ -1632,7 +1642,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A10,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A10,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H10">
@@ -1660,37 +1670,36 @@
         <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E11" s="10">
-        <f>20</f>
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G11">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A11,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A11,'Horas insumidas'!$F$6:$F$135)</f>
         <v>3.5</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>-3.5</v>
+        <v>4.5</v>
       </c>
       <c r="I11">
         <f t="shared" si="1"/>
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.2857142857142856</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1701,37 +1710,36 @@
         <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E12" s="10">
-        <f>20</f>
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G12">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A12,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A12,'Horas insumidas'!$F$6:$F$135)</f>
         <v>5</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>3</v>
       </c>
       <c r="I12">
         <f t="shared" si="1"/>
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="J12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1742,37 +1750,36 @@
         <v>86</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E13" s="10">
-        <f>20</f>
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G13">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A13,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A13,'Horas insumidas'!$F$6:$F$135)</f>
         <v>4.5</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>-4.5</v>
+        <v>3.5</v>
       </c>
       <c r="I13">
         <f t="shared" si="1"/>
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="J13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.7777777777777777</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1783,37 +1790,36 @@
         <v>88</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E14" s="10">
-        <f>20</f>
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G14">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A14,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A14,'Horas insumidas'!$F$6:$F$135)</f>
         <v>2</v>
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>6</v>
       </c>
       <c r="I14">
         <f t="shared" si="1"/>
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1824,37 +1830,36 @@
         <v>89</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D15">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E15" s="10">
-        <f>20</f>
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G15">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A15,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A15,'Horas insumidas'!$F$6:$F$135)</f>
         <v>8</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>0</v>
       </c>
       <c r="I15">
         <f t="shared" si="1"/>
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1878,7 +1883,7 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A16,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A16,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H16">
@@ -1919,7 +1924,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A17,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A17,'Horas insumidas'!$F$6:$F$135)</f>
         <v>0</v>
       </c>
       <c r="H17">
@@ -1947,41 +1952,41 @@
         <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D18">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E18" s="10">
         <f>13</f>
         <v>13</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G18">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A18,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A18,'Horas insumidas'!$F$6:$F$135)</f>
         <v>17.5</v>
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
-        <v>-17.5</v>
+        <v>-4.5</v>
       </c>
       <c r="I18">
         <f t="shared" si="1"/>
-        <v>-13</v>
+        <v>0</v>
       </c>
       <c r="J18">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.74285714285714288</v>
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" t="s">
+      <c r="A19" s="8" t="s">
         <v>112</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -1994,13 +1999,14 @@
         <v>100</v>
       </c>
       <c r="E19" s="10">
+        <f>70</f>
         <v>70</v>
       </c>
       <c r="F19">
         <v>70</v>
       </c>
       <c r="G19">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A19,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A19,'Horas insumidas'!$F$6:$F$135)</f>
         <v>44.5</v>
       </c>
       <c r="H19">
@@ -2021,7 +2027,7 @@
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" t="s">
+      <c r="A20" s="8" t="s">
         <v>119</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -2034,83 +2040,172 @@
         <v>100</v>
       </c>
       <c r="E20" s="10">
+        <f>10</f>
         <v>10</v>
       </c>
       <c r="F20">
         <v>10</v>
       </c>
       <c r="G20">
-        <f ca="1">SUMIF('Horas insumidas'!$E$6:$E$135,A20,'Horas insumidas'!$F$6:$F$135)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A20,'Horas insumidas'!$F$6:$F$135)</f>
         <v>2</v>
       </c>
       <c r="H20">
-        <f t="shared" si="0"/>
+        <f>F20-G20</f>
         <v>8</v>
       </c>
       <c r="I20">
-        <f t="shared" si="1"/>
+        <f>F20-E20</f>
         <v>0</v>
       </c>
       <c r="J20">
-        <f t="shared" si="2"/>
+        <f>F20/E20</f>
         <v>1</v>
       </c>
       <c r="K20">
-        <f t="shared" si="3"/>
+        <f>F20/G20</f>
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" t="s">
-        <v>69</v>
+      <c r="A21" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C21" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21">
+        <v>50</v>
+      </c>
+      <c r="E21" s="10">
+        <v>29</v>
+      </c>
+      <c r="F21">
+        <v>15</v>
+      </c>
+      <c r="G21">
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A21,'Horas insumidas'!$F$6:$F$135)</f>
+        <v>15</v>
+      </c>
+      <c r="H21">
+        <f>F21-G21</f>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f>F21-E21</f>
+        <v>-14</v>
+      </c>
+      <c r="J21">
+        <f>F21/E21</f>
+        <v>0.51724137931034486</v>
+      </c>
+      <c r="K21">
+        <f>F21/G21</f>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" t="s">
-        <v>103</v>
+        <v>151</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22">
+        <v>50</v>
+      </c>
+      <c r="E22" s="10">
+        <v>15</v>
+      </c>
+      <c r="F22">
+        <v>7</v>
+      </c>
+      <c r="G22">
+        <f>SUMIF('Horas insumidas'!$E$6:$E$135,A22,'Horas insumidas'!$F$6:$F$135)</f>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f>F22-G22</f>
+        <v>7</v>
+      </c>
+      <c r="I22">
+        <f>F22-E22</f>
+        <v>-8</v>
+      </c>
+      <c r="J22">
+        <f>F22/E22</f>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="K22" t="e">
+        <f>F22/G22</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B25" s="8" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
-      <c r="D24" t="s">
+    <row r="26" spans="1:11">
+      <c r="A26" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="D27" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="9">
-        <f>SUM(E2:E20)</f>
-        <v>533</v>
-      </c>
-      <c r="F24">
-        <f>SUM(F2:F20)</f>
-        <v>120</v>
-      </c>
-      <c r="G24">
-        <f>SUM(G2:G20)</f>
-        <v>162</v>
-      </c>
-      <c r="H24">
-        <f>SUM(H2:H20)</f>
-        <v>-42</v>
-      </c>
-      <c r="I24">
-        <f>SUM(I2:I20)</f>
-        <v>-413</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="B27" s="2"/>
+      <c r="E27" s="9">
+        <f>SUM(E2:E21)</f>
+        <v>442</v>
+      </c>
+      <c r="F27">
+        <f>SUM(F2:F21)</f>
+        <v>248</v>
+      </c>
+      <c r="G27">
+        <f>SUM(G2:G21)</f>
+        <v>177</v>
+      </c>
+      <c r="H27">
+        <f>SUM(H2:H21)</f>
+        <v>71</v>
+      </c>
+      <c r="I27">
+        <f>SUM(I2:I21)</f>
+        <v>-194</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="B30" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2122,8 +2217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F137"/>
   <sheetViews>
-    <sheetView topLeftCell="B111" workbookViewId="0">
-      <selection activeCell="F138" sqref="F138"/>
+    <sheetView topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="F128" sqref="F128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3798,70 +3893,70 @@
     </row>
     <row r="114" spans="2:6">
       <c r="B114" s="1">
-        <v>40485</v>
+        <v>40484</v>
       </c>
       <c r="C114" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="D114" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E114" t="s">
-        <v>141</v>
+        <v>87</v>
       </c>
       <c r="F114">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="2:6">
       <c r="B115" s="1">
-        <v>40486</v>
+        <v>40484</v>
       </c>
       <c r="C115" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="D115" t="s">
-        <v>142</v>
-      </c>
-      <c r="E115" t="s">
-        <v>141</v>
+        <v>144</v>
+      </c>
+      <c r="E115" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="F115">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="2:6">
       <c r="B116" s="1">
-        <v>40484</v>
+        <v>40485</v>
       </c>
       <c r="C116" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="D116" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="E116" t="s">
-        <v>87</v>
+        <v>141</v>
       </c>
       <c r="F116">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117" spans="2:6">
       <c r="B117" s="1">
-        <v>40484</v>
+        <v>40485</v>
       </c>
       <c r="C117" t="s">
-        <v>95</v>
+        <v>33</v>
       </c>
       <c r="D117" t="s">
-        <v>144</v>
-      </c>
-      <c r="E117" s="8" t="s">
-        <v>14</v>
+        <v>140</v>
+      </c>
+      <c r="E117" t="s">
+        <v>141</v>
       </c>
       <c r="F117">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118" spans="2:6">
@@ -3900,19 +3995,42 @@
     </row>
     <row r="120" spans="2:6">
       <c r="B120" s="1">
+        <v>40486</v>
+      </c>
+      <c r="C120" t="s">
+        <v>33</v>
+      </c>
+      <c r="D120" t="s">
+        <v>142</v>
+      </c>
+      <c r="E120" t="s">
+        <v>141</v>
+      </c>
+      <c r="F120">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="2:6">
+      <c r="B121" s="1">
         <v>40489</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C121" t="s">
         <v>95</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D121" t="s">
         <v>53</v>
       </c>
-      <c r="E120" t="s">
+      <c r="E121" t="s">
         <v>146</v>
       </c>
-      <c r="F120">
+      <c r="F121">
         <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="2:6">
+      <c r="F127">
+        <f>SUM(F114:F126)</f>
+        <v>22</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -3923,8 +4041,8 @@
         <v>147</v>
       </c>
       <c r="F137" s="3">
-        <f>SUM(F114:F136)</f>
-        <v>17</v>
+        <f>SUM(F116:F136)</f>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3945,7 +4063,7 @@
   <dimension ref="B19:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3983,15 +4101,15 @@
         <v>46</v>
       </c>
       <c r="C20" s="11">
-        <f ca="1">'Earned Value'!E2</f>
+        <f>'Earned Value'!E2</f>
         <v>40</v>
       </c>
       <c r="D20" s="11">
-        <f ca="1">'Earned Value'!F2</f>
+        <f>'Earned Value'!F2</f>
         <v>40</v>
       </c>
       <c r="E20" s="11">
-        <f ca="1">'Earned Value'!G2</f>
+        <f>'Earned Value'!G2</f>
         <v>33.5</v>
       </c>
       <c r="F20" s="11">
@@ -4076,29 +4194,29 @@
         <v>63</v>
       </c>
       <c r="C23" s="11">
-        <v>233</v>
+        <v>285</v>
       </c>
       <c r="D23" s="11">
-        <v>190</v>
+        <v>216</v>
       </c>
       <c r="E23" s="11">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="F23" s="11">
         <f>D23-E23</f>
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G23" s="11">
         <f>D23-C23</f>
-        <v>-43</v>
+        <v>-69</v>
       </c>
       <c r="H23" s="11">
         <f>D23/C23</f>
-        <v>0.81545064377682408</v>
+        <v>0.75789473684210529</v>
       </c>
       <c r="I23" s="11">
         <f>D23/E23</f>
-        <v>1.027027027027027</v>
+        <v>1.1076923076923078</v>
       </c>
     </row>
     <row r="24" spans="2:9">
@@ -4107,7 +4225,7 @@
       </c>
       <c r="C24" s="11">
         <f>C23+40</f>
-        <v>273</v>
+        <v>325</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
@@ -4117,7 +4235,7 @@
       </c>
       <c r="G24" s="11">
         <f>D24-C24</f>
-        <v>-273</v>
+        <v>-325</v>
       </c>
       <c r="H24" s="11">
         <f>D24/C24</f>

</xml_diff>

<commit_message>
S-01006 - Horas insumidas del commit anterior
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Earned Value" sheetId="1" r:id="rId1"/>
     <sheet name="Horas insumidas" sheetId="2" r:id="rId2"/>
     <sheet name="Estadísticas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="155">
   <si>
     <t>Id</t>
   </si>
@@ -478,13 +478,16 @@
   </si>
   <si>
     <t>Se agregan niveles de seguridad (Agent, Supervisor y AccountManager)</t>
+  </si>
+  <si>
+    <t>Se agregan metricas de campaña para supervisores junto con graficos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -615,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -646,6 +649,9 @@
     <xf numFmtId="16" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,19 +668,8 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:lang val="es-AR"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -684,12 +679,11 @@
           <c:x val="7.0140280561122259E-2"/>
           <c:y val="4.8611111111111112E-2"/>
           <c:w val="0.70340681362725455"/>
-          <c:h val="0.82986111111111138"/>
+          <c:h val="0.82986111111111149"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -751,7 +745,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -811,7 +804,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -871,31 +863,19 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="104288256"/>
-        <c:axId val="79270400"/>
+        <c:axId val="65889792"/>
+        <c:axId val="65891328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="104288256"/>
+        <c:axId val="65889792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr rot="0" vert="horz"/>
@@ -911,29 +891,25 @@
                 <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79270400"/>
+        <c:crossAx val="65891328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79270400"/>
+        <c:axId val="65891328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104288256"/>
+        <c:crossAx val="65889792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -944,21 +920,19 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86773547094188408"/>
-          <c:y val="0.37152777777777807"/>
-          <c:w val="0.11422845691382745"/>
-          <c:h val="0.24999999999999989"/>
+          <c:x val="0.8677354709418843"/>
+          <c:y val="0.37152777777777818"/>
+          <c:w val="0.11422845691382746"/>
+          <c:h val="0.24999999999999994"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000522" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000522" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000533" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000533" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1076,7 +1050,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1111,7 +1084,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1287,14 +1259,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.85546875" bestFit="1" customWidth="1"/>
@@ -1307,7 +1279,7 @@
     <col min="10" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1342,7 +1314,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
@@ -1383,7 +1355,7 @@
         <v>1.1940298507462686</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
@@ -1423,7 +1395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
@@ -1464,7 +1436,7 @@
         <v>1.9512195121951219</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
@@ -1504,7 +1476,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="8" t="s">
         <v>18</v>
       </c>
@@ -1525,11 +1497,11 @@
       </c>
       <c r="G6">
         <f>SUMIF('Horas insumidas'!$E$6:$E$135,A6,'Horas insumidas'!$F$6:$F$135)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
@@ -1539,12 +1511,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K6" t="e">
+      <c r="K6">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="8" t="s">
         <v>20</v>
       </c>
@@ -1585,7 +1557,7 @@
         <v>0.95238095238095233</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="8" t="s">
         <v>22</v>
       </c>
@@ -1626,7 +1598,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="8" t="s">
         <v>24</v>
       </c>
@@ -1667,7 +1639,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="8" t="s">
         <v>26</v>
       </c>
@@ -1708,7 +1680,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="8" t="s">
         <v>81</v>
       </c>
@@ -1748,7 +1720,7 @@
         <v>2.2857142857142856</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="8" t="s">
         <v>83</v>
       </c>
@@ -1788,7 +1760,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="8" t="s">
         <v>85</v>
       </c>
@@ -1828,7 +1800,7 @@
         <v>1.7777777777777777</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="8" t="s">
         <v>87</v>
       </c>
@@ -1868,7 +1840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="8" t="s">
         <v>75</v>
       </c>
@@ -1908,7 +1880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="8" t="s">
         <v>90</v>
       </c>
@@ -1949,7 +1921,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="8" t="s">
         <v>92</v>
       </c>
@@ -1990,7 +1962,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="8" t="s">
         <v>71</v>
       </c>
@@ -2031,7 +2003,7 @@
         <v>0.74285714285714288</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="8" t="s">
         <v>112</v>
       </c>
@@ -2072,7 +2044,7 @@
         <v>1.5730337078651686</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="8" t="s">
         <v>119</v>
       </c>
@@ -2113,7 +2085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="8" t="s">
         <v>141</v>
       </c>
@@ -2153,7 +2125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="8" t="s">
         <v>151</v>
       </c>
@@ -2193,7 +2165,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="8" t="s">
         <v>68</v>
       </c>
@@ -2201,7 +2173,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="8" t="s">
         <v>102</v>
       </c>
@@ -2209,7 +2181,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="8" t="s">
         <v>121</v>
       </c>
@@ -2217,7 +2189,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="8" t="s">
         <v>146</v>
       </c>
@@ -2225,7 +2197,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="D27" t="s">
         <v>28</v>
       </c>
@@ -2239,18 +2211,18 @@
       </c>
       <c r="G27">
         <f>SUM(G2:G21)</f>
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="H27">
         <f>SUM(H2:H21)</f>
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I27">
         <f>SUM(I2:I21)</f>
         <v>-184</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="B30" s="2"/>
     </row>
   </sheetData>
@@ -2260,14 +2232,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F137"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="H119" sqref="H119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
@@ -2276,8 +2248,8 @@
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:6" ht="15.75" thickBot="1">
       <c r="B2" s="4" t="s">
         <v>29</v>
       </c>
@@ -2294,7 +2266,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6">
       <c r="B3" s="1">
         <v>40428</v>
       </c>
@@ -2308,7 +2280,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6">
       <c r="B4" s="1">
         <v>40429</v>
       </c>
@@ -2322,7 +2294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6">
       <c r="B5" s="1">
         <v>40429</v>
       </c>
@@ -2336,7 +2308,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6">
       <c r="B6" s="1">
         <v>40431</v>
       </c>
@@ -2350,7 +2322,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6">
       <c r="B7" s="1">
         <v>40432</v>
       </c>
@@ -2364,7 +2336,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6">
       <c r="B8" s="1">
         <v>40432</v>
       </c>
@@ -2378,7 +2350,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6">
       <c r="B9" s="1">
         <v>40432</v>
       </c>
@@ -2392,7 +2364,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6">
       <c r="B10" s="1">
         <v>40432</v>
       </c>
@@ -2406,7 +2378,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6">
       <c r="B11" s="1">
         <v>40433</v>
       </c>
@@ -2420,7 +2392,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6">
       <c r="B12" s="13" t="s">
         <v>46</v>
       </c>
@@ -2429,7 +2401,7 @@
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6">
       <c r="B13" s="1">
         <v>40435</v>
       </c>
@@ -2446,7 +2418,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6">
       <c r="B14" s="1">
         <v>40435</v>
       </c>
@@ -2463,7 +2435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6">
       <c r="B15" s="1">
         <v>40435</v>
       </c>
@@ -2480,7 +2452,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6">
       <c r="B16" s="1">
         <v>40435</v>
       </c>
@@ -2497,7 +2469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6">
       <c r="B17" s="1">
         <v>40435</v>
       </c>
@@ -2514,7 +2486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6">
       <c r="B18" s="1">
         <v>40435</v>
       </c>
@@ -2531,7 +2503,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6">
       <c r="B19" s="1">
         <v>40436</v>
       </c>
@@ -2548,7 +2520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6">
       <c r="B20" s="1">
         <v>40436</v>
       </c>
@@ -2565,7 +2537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6">
       <c r="B21" s="1">
         <v>40436</v>
       </c>
@@ -2582,7 +2554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6">
       <c r="B22" s="1">
         <v>40437</v>
       </c>
@@ -2599,7 +2571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6">
       <c r="B23" s="1">
         <v>40438</v>
       </c>
@@ -2616,7 +2588,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6">
       <c r="B24" s="1">
         <v>40439</v>
       </c>
@@ -2633,7 +2605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6">
       <c r="B25" s="1">
         <v>40439</v>
       </c>
@@ -2650,7 +2622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6">
       <c r="B26" s="1">
         <v>40439</v>
       </c>
@@ -2667,7 +2639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6">
       <c r="B27" s="1">
         <v>40441</v>
       </c>
@@ -2684,7 +2656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6">
       <c r="B28" s="1">
         <v>40442</v>
       </c>
@@ -2701,7 +2673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6">
       <c r="B29" s="1">
         <v>40442</v>
       </c>
@@ -2718,7 +2690,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6">
       <c r="B30" s="1">
         <v>40442</v>
       </c>
@@ -2735,7 +2707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6">
       <c r="B31" s="1">
         <v>40442</v>
       </c>
@@ -2752,7 +2724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6">
       <c r="B32" s="1">
         <v>40444</v>
       </c>
@@ -2769,7 +2741,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6">
       <c r="B33" s="1">
         <v>40444</v>
       </c>
@@ -2786,7 +2758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6">
       <c r="B34" s="1">
         <v>40444</v>
       </c>
@@ -2803,7 +2775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6">
       <c r="B35" s="1">
         <v>40444</v>
       </c>
@@ -2820,7 +2792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6">
       <c r="B36" s="1">
         <v>40445</v>
       </c>
@@ -2837,7 +2809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6">
       <c r="B37" s="1">
         <v>40445</v>
       </c>
@@ -2854,7 +2826,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6">
       <c r="B38" s="1">
         <v>40445</v>
       </c>
@@ -2871,7 +2843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6">
       <c r="B39" s="1">
         <v>40445</v>
       </c>
@@ -2888,7 +2860,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6">
       <c r="B40" s="1">
         <v>40446</v>
       </c>
@@ -2905,7 +2877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6">
       <c r="B41" s="1">
         <v>40448</v>
       </c>
@@ -2922,7 +2894,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -2934,7 +2906,7 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6">
       <c r="B43" s="13" t="s">
         <v>61</v>
       </c>
@@ -2943,7 +2915,7 @@
       <c r="E43" s="13"/>
       <c r="F43" s="13"/>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6">
       <c r="B44" s="1">
         <v>40450</v>
       </c>
@@ -2960,7 +2932,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:6">
       <c r="B45" s="1">
         <v>40450</v>
       </c>
@@ -2977,7 +2949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:6">
       <c r="B46" s="1">
         <v>40450</v>
       </c>
@@ -2994,7 +2966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:6">
       <c r="B47" s="1">
         <v>40451</v>
       </c>
@@ -3011,7 +2983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:6">
       <c r="B48" s="1">
         <v>40452</v>
       </c>
@@ -3028,7 +3000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:6">
       <c r="B49" s="1">
         <v>40453</v>
       </c>
@@ -3045,7 +3017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:6" ht="17.25" customHeight="1">
       <c r="B50" s="1">
         <v>40452</v>
       </c>
@@ -3062,7 +3034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:6" ht="30">
       <c r="B51" s="1">
         <v>40453</v>
       </c>
@@ -3079,7 +3051,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:6" ht="18" customHeight="1">
       <c r="B52" s="1">
         <v>40454</v>
       </c>
@@ -3096,7 +3068,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:6">
       <c r="B53" s="1">
         <v>40454</v>
       </c>
@@ -3113,7 +3085,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:6">
       <c r="B54" s="1">
         <v>40454</v>
       </c>
@@ -3130,7 +3102,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:6">
       <c r="B55" s="1">
         <v>40454</v>
       </c>
@@ -3147,7 +3119,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:6">
       <c r="B56" s="1">
         <v>40455</v>
       </c>
@@ -3164,7 +3136,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:6">
       <c r="B57" s="1">
         <v>40455</v>
       </c>
@@ -3181,7 +3153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:6">
       <c r="B58" s="1">
         <v>40456</v>
       </c>
@@ -3198,7 +3170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:6">
       <c r="B59" s="1">
         <v>40456</v>
       </c>
@@ -3215,7 +3187,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:6">
       <c r="B60" s="1">
         <v>40457</v>
       </c>
@@ -3232,7 +3204,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:6">
       <c r="B61" s="1">
         <v>40458</v>
       </c>
@@ -3249,7 +3221,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:6">
       <c r="B62" s="1">
         <v>40459</v>
       </c>
@@ -3266,7 +3238,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:6">
       <c r="B63" s="1">
         <v>40460</v>
       </c>
@@ -3283,7 +3255,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:6">
       <c r="B64" s="1">
         <v>40462</v>
       </c>
@@ -3300,7 +3272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:6">
       <c r="B65" s="1">
         <v>40463</v>
       </c>
@@ -3317,7 +3289,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:6">
       <c r="B66" s="1">
         <v>40464</v>
       </c>
@@ -3334,7 +3306,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:6">
       <c r="B67" s="1">
         <v>40465</v>
       </c>
@@ -3351,7 +3323,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:6">
       <c r="B68" s="1">
         <v>40465</v>
       </c>
@@ -3368,7 +3340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:6">
       <c r="B69" s="1">
         <v>40465</v>
       </c>
@@ -3385,7 +3357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:6">
       <c r="B70" s="1">
         <v>40465</v>
       </c>
@@ -3402,7 +3374,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:6">
       <c r="B71" s="1">
         <v>40466</v>
       </c>
@@ -3419,7 +3391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:6">
       <c r="B72" s="1">
         <v>40467</v>
       </c>
@@ -3436,7 +3408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:6">
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
@@ -3448,7 +3420,7 @@
         <v>66.5</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:6">
       <c r="B81" s="13" t="s">
         <v>62</v>
       </c>
@@ -3457,7 +3429,7 @@
       <c r="E81" s="13"/>
       <c r="F81" s="13"/>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:6">
       <c r="B82" s="1">
         <v>40471</v>
       </c>
@@ -3474,7 +3446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:6">
       <c r="B83" s="1">
         <v>40471</v>
       </c>
@@ -3491,7 +3463,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:6">
       <c r="B84" s="1">
         <v>40472</v>
       </c>
@@ -3508,7 +3480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:6">
       <c r="B85" s="1">
         <v>40472</v>
       </c>
@@ -3525,7 +3497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:6">
       <c r="B86" s="1">
         <v>40472</v>
       </c>
@@ -3542,7 +3514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:6">
       <c r="B87" s="1">
         <v>40472</v>
       </c>
@@ -3559,7 +3531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:6">
       <c r="B88" s="1">
         <v>40473</v>
       </c>
@@ -3576,7 +3548,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:6">
       <c r="B89" s="1">
         <v>40474</v>
       </c>
@@ -3593,7 +3565,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:6">
       <c r="B90" s="1">
         <v>40474</v>
       </c>
@@ -3610,7 +3582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:6">
       <c r="B91" s="1">
         <v>40474</v>
       </c>
@@ -3627,7 +3599,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:6">
       <c r="B92" s="1">
         <v>40474</v>
       </c>
@@ -3644,7 +3616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:6">
       <c r="B93" s="1">
         <v>40474</v>
       </c>
@@ -3661,7 +3633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:6">
       <c r="B94" s="1">
         <v>40475</v>
       </c>
@@ -3678,7 +3650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:6">
       <c r="B95" s="1">
         <v>40475</v>
       </c>
@@ -3695,7 +3667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:6">
       <c r="B96" s="1">
         <v>40475</v>
       </c>
@@ -3712,7 +3684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:6">
       <c r="B97" s="1">
         <v>40475</v>
       </c>
@@ -3729,7 +3701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:6">
       <c r="B98" s="1">
         <v>40476</v>
       </c>
@@ -3746,7 +3718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:6">
       <c r="B99" s="1">
         <v>40478</v>
       </c>
@@ -3763,7 +3735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:6">
       <c r="B100" s="1">
         <v>40478</v>
       </c>
@@ -3780,7 +3752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:6">
       <c r="B101" s="1">
         <v>40478</v>
       </c>
@@ -3797,7 +3769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:6">
       <c r="B102" s="1">
         <v>40478</v>
       </c>
@@ -3814,7 +3786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:6">
       <c r="B103" s="1">
         <v>40481</v>
       </c>
@@ -3831,7 +3803,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:6">
       <c r="B104" s="1">
         <v>40482</v>
       </c>
@@ -3848,7 +3820,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:6">
       <c r="B105" s="1">
         <v>40482</v>
       </c>
@@ -3865,7 +3837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:6">
       <c r="B106" s="1">
         <v>40482</v>
       </c>
@@ -3882,7 +3854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:6">
       <c r="B107" s="1">
         <v>40482</v>
       </c>
@@ -3899,7 +3871,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:6">
       <c r="B108" s="1">
         <v>40482</v>
       </c>
@@ -3916,7 +3888,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:6">
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
@@ -3928,7 +3900,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:6">
       <c r="B113" s="13" t="s">
         <v>63</v>
       </c>
@@ -3937,7 +3909,7 @@
       <c r="E113" s="13"/>
       <c r="F113" s="13"/>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:6">
       <c r="B114" s="1">
         <v>40484</v>
       </c>
@@ -3954,7 +3926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:6">
       <c r="B115" s="1">
         <v>40484</v>
       </c>
@@ -3971,7 +3943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:6">
       <c r="B116" s="1">
         <v>40485</v>
       </c>
@@ -3988,7 +3960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:6">
       <c r="B117" s="1">
         <v>40485</v>
       </c>
@@ -4005,7 +3977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:6">
       <c r="B118" s="1">
         <v>40485</v>
       </c>
@@ -4022,7 +3994,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:6">
       <c r="B119" s="1">
         <v>40485</v>
       </c>
@@ -4039,7 +4011,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:6">
       <c r="B120" s="1">
         <v>40486</v>
       </c>
@@ -4056,7 +4028,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:6">
       <c r="B121" s="1">
         <v>40489</v>
       </c>
@@ -4073,7 +4045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:6">
       <c r="B122" s="1">
         <v>40491</v>
       </c>
@@ -4090,18 +4062,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B123" s="12"/>
-      <c r="C123" s="12"/>
-      <c r="E123" s="12"/>
-    </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F127">
-        <f>SUM(F114:F126)</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:6">
+      <c r="B123" s="14">
+        <v>40492</v>
+      </c>
+      <c r="C123" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D123" t="s">
+        <v>154</v>
+      </c>
+      <c r="E123" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F123">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="2:6">
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
       <c r="D137" s="3"/>
@@ -4109,8 +4087,8 @@
         <v>147</v>
       </c>
       <c r="F137" s="3">
-        <f>SUM(F116:F136)</f>
-        <v>50</v>
+        <f>SUM(F114:F136)</f>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -4127,20 +4105,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B19:I24"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9">
       <c r="B19" s="11"/>
       <c r="C19" s="11" t="s">
         <v>3</v>
@@ -4164,7 +4142,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9">
       <c r="B20" s="11" t="s">
         <v>46</v>
       </c>
@@ -4197,7 +4175,7 @@
         <v>1.1940298507462686</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9">
       <c r="B21" s="11" t="s">
         <v>61</v>
       </c>
@@ -4227,7 +4205,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9">
       <c r="B22" s="11" t="s">
         <v>62</v>
       </c>
@@ -4257,7 +4235,7 @@
         <v>0.93865030674846628</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9">
       <c r="B23" s="11" t="s">
         <v>63</v>
       </c>
@@ -4287,7 +4265,7 @@
         <v>1.1076923076923078</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9">
       <c r="B24" s="11" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
Se modifican querys de init.sql
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Earned Value" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="161">
   <si>
     <t>Id</t>
   </si>
@@ -496,6 +496,9 @@
   </si>
   <si>
     <t>Se quita el campo valor hora no satisfactorio (vale siempre $0)</t>
+  </si>
+  <si>
+    <t>Se configuran archivos de prueba para todo el sistema</t>
   </si>
 </sst>
 </file>
@@ -887,11 +890,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84159488"/>
-        <c:axId val="84173568"/>
+        <c:axId val="77549568"/>
+        <c:axId val="77551104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84159488"/>
+        <c:axId val="77549568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -915,14 +918,14 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84173568"/>
+        <c:crossAx val="77551104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84173568"/>
+        <c:axId val="77551104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -930,7 +933,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84159488"/>
+        <c:crossAx val="77549568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -941,8 +944,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86773547094188486"/>
-          <c:y val="0.37152777777777857"/>
+          <c:x val="0.86773547094188508"/>
+          <c:y val="0.37152777777777868"/>
           <c:w val="0.11422845691382746"/>
           <c:h val="0.25"/>
         </c:manualLayout>
@@ -953,7 +956,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000566" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000566" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000577" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000577" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1518,11 +1521,11 @@
       </c>
       <c r="G6">
         <f>SUMIF('Horas insumidas'!$E$6:$E$139,A6,'Horas insumidas'!$F$6:$F$139)</f>
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
@@ -1534,7 +1537,7 @@
       </c>
       <c r="K6">
         <f t="shared" si="3"/>
-        <v>1.6666666666666667</v>
+        <v>1.0526315789473684</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -2232,11 +2235,11 @@
       </c>
       <c r="G27">
         <f>SUM(G2:G21)</f>
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="H27">
         <f>SUM(H2:H21)</f>
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I27">
         <f>SUM(I2:I21)</f>
@@ -2256,8 +2259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F141"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="E123" sqref="E123"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4219,6 +4222,23 @@
         <v>2</v>
       </c>
     </row>
+    <row r="131" spans="2:6">
+      <c r="B131" s="1">
+        <v>40496</v>
+      </c>
+      <c r="C131" t="s">
+        <v>47</v>
+      </c>
+      <c r="D131" t="s">
+        <v>160</v>
+      </c>
+      <c r="E131" t="s">
+        <v>18</v>
+      </c>
+      <c r="F131">
+        <v>7</v>
+      </c>
+    </row>
     <row r="141" spans="2:6">
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
@@ -4228,7 +4248,7 @@
       </c>
       <c r="F141" s="3">
         <f>SUM(F114:F140)</f>
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -4248,7 +4268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B19:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
S-01026 - Se mejora la visualizacion de los graficos de totales supervisor
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="164">
   <si>
     <t>Id</t>
   </si>
@@ -499,6 +499,15 @@
   </si>
   <si>
     <t>Se configuran archivos de prueba para todo el sistema</t>
+  </si>
+  <si>
+    <t>Total Sprint 5</t>
+  </si>
+  <si>
+    <t>Se mejora la visualizacion de totales supervisor</t>
+  </si>
+  <si>
+    <t>S-01026</t>
   </si>
 </sst>
 </file>
@@ -890,11 +899,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77549568"/>
-        <c:axId val="77551104"/>
+        <c:axId val="59260928"/>
+        <c:axId val="59262464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77549568"/>
+        <c:axId val="59260928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -918,14 +927,14 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77551104"/>
+        <c:crossAx val="59262464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77551104"/>
+        <c:axId val="59262464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -933,7 +942,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77549568"/>
+        <c:crossAx val="59260928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -944,8 +953,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86773547094188508"/>
-          <c:y val="0.37152777777777868"/>
+          <c:x val="0.8677354709418853"/>
+          <c:y val="0.37152777777777879"/>
           <c:w val="0.11422845691382746"/>
           <c:h val="0.25"/>
         </c:manualLayout>
@@ -956,7 +965,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000577" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000577" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000588" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000588" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1359,7 +1368,7 @@
         <v>40</v>
       </c>
       <c r="G2">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A2,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A2,'Horas insumidas'!$F$6:$F$131)</f>
         <v>33.5</v>
       </c>
       <c r="H2">
@@ -1399,7 +1408,7 @@
         <v>20</v>
       </c>
       <c r="G3">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A3,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A3,'Horas insumidas'!$F$6:$F$131)</f>
         <v>15</v>
       </c>
       <c r="H3">
@@ -1440,7 +1449,7 @@
         <v>40</v>
       </c>
       <c r="G4">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A4,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A4,'Horas insumidas'!$F$6:$F$131)</f>
         <v>20.5</v>
       </c>
       <c r="H4">
@@ -1480,7 +1489,7 @@
         <v>20</v>
       </c>
       <c r="G5">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A5,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A5,'Horas insumidas'!$F$6:$F$131)</f>
         <v>4</v>
       </c>
       <c r="H5">
@@ -1520,7 +1529,7 @@
         <v>20</v>
       </c>
       <c r="G6">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A6,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A6,'Horas insumidas'!$F$6:$F$131)</f>
         <v>19</v>
       </c>
       <c r="H6">
@@ -1561,7 +1570,7 @@
         <v>20</v>
       </c>
       <c r="G7">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A7,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A7,'Horas insumidas'!$F$6:$F$131)</f>
         <v>21</v>
       </c>
       <c r="H7">
@@ -1602,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A8,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A8,'Horas insumidas'!$F$6:$F$131)</f>
         <v>0</v>
       </c>
       <c r="H8">
@@ -1643,7 +1652,7 @@
         <v>40</v>
       </c>
       <c r="G9">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A9,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A9,'Horas insumidas'!$F$6:$F$131)</f>
         <v>0</v>
       </c>
       <c r="H9">
@@ -1684,7 +1693,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A10,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A10,'Horas insumidas'!$F$6:$F$131)</f>
         <v>0</v>
       </c>
       <c r="H10">
@@ -1724,7 +1733,7 @@
         <v>8</v>
       </c>
       <c r="G11">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A11,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A11,'Horas insumidas'!$F$6:$F$131)</f>
         <v>3.5</v>
       </c>
       <c r="H11">
@@ -1764,7 +1773,7 @@
         <v>8</v>
       </c>
       <c r="G12">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A12,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A12,'Horas insumidas'!$F$6:$F$131)</f>
         <v>5</v>
       </c>
       <c r="H12">
@@ -1804,7 +1813,7 @@
         <v>8</v>
       </c>
       <c r="G13">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A13,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A13,'Horas insumidas'!$F$6:$F$131)</f>
         <v>4.5</v>
       </c>
       <c r="H13">
@@ -1844,7 +1853,7 @@
         <v>8</v>
       </c>
       <c r="G14">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A14,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A14,'Horas insumidas'!$F$6:$F$131)</f>
         <v>2</v>
       </c>
       <c r="H14">
@@ -1884,7 +1893,7 @@
         <v>8</v>
       </c>
       <c r="G15">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A15,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A15,'Horas insumidas'!$F$6:$F$131)</f>
         <v>8</v>
       </c>
       <c r="H15">
@@ -1925,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A16,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A16,'Horas insumidas'!$F$6:$F$131)</f>
         <v>0</v>
       </c>
       <c r="H16">
@@ -1966,7 +1975,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A17,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A17,'Horas insumidas'!$F$6:$F$131)</f>
         <v>0</v>
       </c>
       <c r="H17">
@@ -2007,7 +2016,7 @@
         <v>13</v>
       </c>
       <c r="G18">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A18,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A18,'Horas insumidas'!$F$6:$F$131)</f>
         <v>17.5</v>
       </c>
       <c r="H18">
@@ -2048,7 +2057,7 @@
         <v>70</v>
       </c>
       <c r="G19">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A19,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A19,'Horas insumidas'!$F$6:$F$131)</f>
         <v>44.5</v>
       </c>
       <c r="H19">
@@ -2089,7 +2098,7 @@
         <v>10</v>
       </c>
       <c r="G20">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A20,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A20,'Horas insumidas'!$F$6:$F$131)</f>
         <v>2</v>
       </c>
       <c r="H20">
@@ -2129,7 +2138,7 @@
         <v>29</v>
       </c>
       <c r="G21">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A21,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A21,'Horas insumidas'!$F$6:$F$131)</f>
         <v>19</v>
       </c>
       <c r="H21">
@@ -2169,7 +2178,7 @@
         <v>7</v>
       </c>
       <c r="G22">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$139,A22,'Horas insumidas'!$F$6:$F$139)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A22,'Horas insumidas'!$F$6:$F$131)</f>
         <v>0</v>
       </c>
       <c r="H22">
@@ -2257,10 +2266,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F141"/>
+  <dimension ref="B1:F163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4239,24 +4248,63 @@
         <v>7</v>
       </c>
     </row>
-    <row r="141" spans="2:6">
-      <c r="B141" s="3"/>
-      <c r="C141" s="3"/>
-      <c r="D141" s="3"/>
-      <c r="E141" s="3" t="s">
+    <row r="132" spans="2:6">
+      <c r="B132" s="3"/>
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="F141" s="3">
-        <f>SUM(F114:F140)</f>
+      <c r="F132" s="3">
+        <f>SUM(F114:F131)</f>
         <v>64</v>
       </c>
     </row>
+    <row r="134" spans="2:6">
+      <c r="B134" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C134" s="15"/>
+      <c r="D134" s="15"/>
+      <c r="E134" s="15"/>
+      <c r="F134" s="15"/>
+    </row>
+    <row r="135" spans="2:6">
+      <c r="B135" s="1">
+        <v>40500</v>
+      </c>
+      <c r="C135" t="s">
+        <v>47</v>
+      </c>
+      <c r="D135" t="s">
+        <v>162</v>
+      </c>
+      <c r="E135" t="s">
+        <v>163</v>
+      </c>
+      <c r="F135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="2:6">
+      <c r="B163" s="3"/>
+      <c r="C163" s="3"/>
+      <c r="D163" s="3"/>
+      <c r="E163" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F163" s="3">
+        <f>SUM(F135:F162)</f>
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B43:F43"/>
     <mergeCell ref="B81:F81"/>
     <mergeCell ref="B113:F113"/>
+    <mergeCell ref="B134:F134"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
S-01030: se corrige el bug de prioridad media (validación de los rangos de las métricas). Cambio de posición el label usuario logueado y rol...
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Earned Value" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="167">
   <si>
     <t>Id</t>
   </si>
@@ -471,9 +471,6 @@
     <t>Correcciones sprint 3</t>
   </si>
   <si>
-    <t>S01024</t>
-  </si>
-  <si>
     <t>Métricas para agentes: 3 métricas</t>
   </si>
   <si>
@@ -508,6 +505,18 @@
   </si>
   <si>
     <t>S-01026</t>
+  </si>
+  <si>
+    <t>S-01030</t>
+  </si>
+  <si>
+    <t>Se corrige el bug de prioridad media de validación de rangos para las métricas</t>
+  </si>
+  <si>
+    <t>S-01024</t>
+  </si>
+  <si>
+    <t>Arreglar todos los bugs de prioridad media/alta que figuran en el informe de avance</t>
   </si>
 </sst>
 </file>
@@ -899,11 +908,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="59260928"/>
-        <c:axId val="59262464"/>
+        <c:axId val="87501824"/>
+        <c:axId val="87520000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="59260928"/>
+        <c:axId val="87501824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -927,14 +936,14 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59262464"/>
+        <c:crossAx val="87520000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59262464"/>
+        <c:axId val="87520000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -942,7 +951,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59260928"/>
+        <c:crossAx val="87501824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -953,8 +962,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.8677354709418853"/>
-          <c:y val="0.37152777777777879"/>
+          <c:x val="0.86773547094188574"/>
+          <c:y val="0.37152777777777907"/>
           <c:w val="0.11422845691382746"/>
           <c:h val="0.25"/>
         </c:manualLayout>
@@ -965,7 +974,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000588" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000588" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000611" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000611" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1293,10 +1302,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1368,7 +1377,7 @@
         <v>40</v>
       </c>
       <c r="G2">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A2,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A2,'Horas insumidas'!$F$6:$F$150)</f>
         <v>33.5</v>
       </c>
       <c r="H2">
@@ -1408,7 +1417,7 @@
         <v>20</v>
       </c>
       <c r="G3">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A3,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A3,'Horas insumidas'!$F$6:$F$150)</f>
         <v>15</v>
       </c>
       <c r="H3">
@@ -1449,7 +1458,7 @@
         <v>40</v>
       </c>
       <c r="G4">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A4,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A4,'Horas insumidas'!$F$6:$F$150)</f>
         <v>20.5</v>
       </c>
       <c r="H4">
@@ -1489,7 +1498,7 @@
         <v>20</v>
       </c>
       <c r="G5">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A5,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A5,'Horas insumidas'!$F$6:$F$150)</f>
         <v>4</v>
       </c>
       <c r="H5">
@@ -1529,7 +1538,7 @@
         <v>20</v>
       </c>
       <c r="G6">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A6,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A6,'Horas insumidas'!$F$6:$F$150)</f>
         <v>19</v>
       </c>
       <c r="H6">
@@ -1570,7 +1579,7 @@
         <v>20</v>
       </c>
       <c r="G7">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A7,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A7,'Horas insumidas'!$F$6:$F$150)</f>
         <v>21</v>
       </c>
       <c r="H7">
@@ -1611,7 +1620,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A8,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A8,'Horas insumidas'!$F$6:$F$150)</f>
         <v>0</v>
       </c>
       <c r="H8">
@@ -1652,7 +1661,7 @@
         <v>40</v>
       </c>
       <c r="G9">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A9,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A9,'Horas insumidas'!$F$6:$F$150)</f>
         <v>0</v>
       </c>
       <c r="H9">
@@ -1693,7 +1702,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A10,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A10,'Horas insumidas'!$F$6:$F$150)</f>
         <v>0</v>
       </c>
       <c r="H10">
@@ -1733,7 +1742,7 @@
         <v>8</v>
       </c>
       <c r="G11">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A11,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A11,'Horas insumidas'!$F$6:$F$150)</f>
         <v>3.5</v>
       </c>
       <c r="H11">
@@ -1773,7 +1782,7 @@
         <v>8</v>
       </c>
       <c r="G12">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A12,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A12,'Horas insumidas'!$F$6:$F$150)</f>
         <v>5</v>
       </c>
       <c r="H12">
@@ -1813,7 +1822,7 @@
         <v>8</v>
       </c>
       <c r="G13">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A13,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A13,'Horas insumidas'!$F$6:$F$150)</f>
         <v>4.5</v>
       </c>
       <c r="H13">
@@ -1853,7 +1862,7 @@
         <v>8</v>
       </c>
       <c r="G14">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A14,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A14,'Horas insumidas'!$F$6:$F$150)</f>
         <v>2</v>
       </c>
       <c r="H14">
@@ -1893,7 +1902,7 @@
         <v>8</v>
       </c>
       <c r="G15">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A15,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A15,'Horas insumidas'!$F$6:$F$150)</f>
         <v>8</v>
       </c>
       <c r="H15">
@@ -1934,7 +1943,7 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A16,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A16,'Horas insumidas'!$F$6:$F$150)</f>
         <v>0</v>
       </c>
       <c r="H16">
@@ -1975,7 +1984,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A17,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A17,'Horas insumidas'!$F$6:$F$150)</f>
         <v>0</v>
       </c>
       <c r="H17">
@@ -2016,7 +2025,7 @@
         <v>13</v>
       </c>
       <c r="G18">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A18,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A18,'Horas insumidas'!$F$6:$F$150)</f>
         <v>17.5</v>
       </c>
       <c r="H18">
@@ -2057,7 +2066,7 @@
         <v>70</v>
       </c>
       <c r="G19">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A19,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A19,'Horas insumidas'!$F$6:$F$150)</f>
         <v>44.5</v>
       </c>
       <c r="H19">
@@ -2098,7 +2107,7 @@
         <v>10</v>
       </c>
       <c r="G20">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A20,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A20,'Horas insumidas'!$F$6:$F$150)</f>
         <v>2</v>
       </c>
       <c r="H20">
@@ -2138,7 +2147,7 @@
         <v>29</v>
       </c>
       <c r="G21">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A21,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A21,'Horas insumidas'!$F$6:$F$150)</f>
         <v>19</v>
       </c>
       <c r="H21">
@@ -2160,10 +2169,10 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>152</v>
       </c>
       <c r="C22" t="s">
         <v>94</v>
@@ -2178,7 +2187,7 @@
         <v>7</v>
       </c>
       <c r="G22">
-        <f>SUMIF('Horas insumidas'!$E$6:$E$131,A22,'Horas insumidas'!$F$6:$F$131)</f>
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A22,'Horas insumidas'!$F$6:$F$150)</f>
         <v>0</v>
       </c>
       <c r="H22">
@@ -2200,66 +2209,109 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="8" t="s">
-        <v>68</v>
+        <v>163</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>69</v>
+        <v>166</v>
+      </c>
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23">
+        <v>100</v>
+      </c>
+      <c r="E23" s="10">
+        <v>20</v>
+      </c>
+      <c r="F23">
+        <v>20</v>
+      </c>
+      <c r="G23">
+        <f>SUMIF('Horas insumidas'!$E$6:$E$150,A23,'Horas insumidas'!$F$6:$F$150)</f>
+        <v>9</v>
+      </c>
+      <c r="H23">
+        <f>F23-G23</f>
+        <v>11</v>
+      </c>
+      <c r="I23">
+        <f>F23-E23</f>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f>F23/E23</f>
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <f>F23/G23</f>
+        <v>2.2222222222222223</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="8" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="8" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B27" s="8" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
-      <c r="D27" t="s">
+    <row r="28" spans="1:11">
+      <c r="D28" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E28" s="9">
         <f>SUM(E2:E21)</f>
         <v>442</v>
       </c>
-      <c r="F27">
+      <c r="F28">
         <f>SUM(F2:F21)</f>
         <v>362</v>
       </c>
-      <c r="G27">
+      <c r="G28">
         <f>SUM(G2:G21)</f>
         <v>219</v>
       </c>
-      <c r="H27">
+      <c r="H28">
         <f>SUM(H2:H21)</f>
         <v>143</v>
       </c>
-      <c r="I27">
+      <c r="I28">
         <f>SUM(I2:I21)</f>
         <v>-80</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
-      <c r="B30" s="2"/>
+    <row r="31" spans="1:11">
+      <c r="B31" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B23" r:id="rId1" display="https://www1.v1host.com/Team152/assetdetail.v1?oid=Story%3a1191"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2268,8 +2320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="E136" sqref="E136"/>
+    <sheetView topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="B138" sqref="B138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4086,7 +4138,7 @@
         <v>65</v>
       </c>
       <c r="D122" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E122" t="s">
         <v>141</v>
@@ -4103,7 +4155,7 @@
         <v>65</v>
       </c>
       <c r="D123" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E123" t="s">
         <v>11</v>
@@ -4120,7 +4172,7 @@
         <v>47</v>
       </c>
       <c r="D124" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E124" s="12" t="s">
         <v>18</v>
@@ -4137,7 +4189,7 @@
         <v>65</v>
       </c>
       <c r="D125" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E125" t="s">
         <v>11</v>
@@ -4154,7 +4206,7 @@
         <v>33</v>
       </c>
       <c r="D126" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E126" t="s">
         <v>18</v>
@@ -4171,7 +4223,7 @@
         <v>33</v>
       </c>
       <c r="D127" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E127" t="s">
         <v>18</v>
@@ -4188,7 +4240,7 @@
         <v>65</v>
       </c>
       <c r="D128" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E128" t="s">
         <v>11</v>
@@ -4205,7 +4257,7 @@
         <v>33</v>
       </c>
       <c r="D129" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E129" t="s">
         <v>16</v>
@@ -4222,7 +4274,7 @@
         <v>65</v>
       </c>
       <c r="D130" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E130" t="s">
         <v>141</v>
@@ -4239,7 +4291,7 @@
         <v>47</v>
       </c>
       <c r="D131" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E131" t="s">
         <v>18</v>
@@ -4277,13 +4329,47 @@
         <v>47</v>
       </c>
       <c r="D135" t="s">
+        <v>161</v>
+      </c>
+      <c r="E135" t="s">
         <v>162</v>
-      </c>
-      <c r="E135" t="s">
-        <v>163</v>
       </c>
       <c r="F135">
         <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="2:6">
+      <c r="B136" s="1">
+        <v>40501</v>
+      </c>
+      <c r="C136" t="s">
+        <v>65</v>
+      </c>
+      <c r="D136" t="s">
+        <v>164</v>
+      </c>
+      <c r="E136" t="s">
+        <v>163</v>
+      </c>
+      <c r="F136">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="2:6">
+      <c r="B137" s="1">
+        <v>40502</v>
+      </c>
+      <c r="C137" t="s">
+        <v>65</v>
+      </c>
+      <c r="D137" t="s">
+        <v>164</v>
+      </c>
+      <c r="E137" t="s">
+        <v>163</v>
+      </c>
+      <c r="F137">
+        <v>6</v>
       </c>
     </row>
     <row r="163" spans="2:6">
@@ -4291,11 +4377,11 @@
       <c r="C163" s="3"/>
       <c r="D163" s="3"/>
       <c r="E163" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F163" s="3">
         <f>SUM(F135:F162)</f>
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
S-01031 Mejoras en la visualizacion del salario del agente
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Earned Value" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="170">
   <si>
     <t>Id</t>
   </si>
@@ -517,6 +517,15 @@
   </si>
   <si>
     <t>Arreglar todos los bugs de prioridad media/alta que figuran en el informe de avance</t>
+  </si>
+  <si>
+    <t>Mejoras varias de usabilidad y navegabilidad</t>
+  </si>
+  <si>
+    <t>S-01031</t>
+  </si>
+  <si>
+    <t>Mejoras en la visualizacion del salario del agente</t>
   </si>
 </sst>
 </file>
@@ -908,11 +917,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="87501824"/>
-        <c:axId val="87520000"/>
+        <c:axId val="66076672"/>
+        <c:axId val="66078208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87501824"/>
+        <c:axId val="66076672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,14 +945,14 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87520000"/>
+        <c:crossAx val="66078208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87520000"/>
+        <c:axId val="66078208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -951,7 +960,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87501824"/>
+        <c:crossAx val="66076672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -962,8 +971,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86773547094188574"/>
-          <c:y val="0.37152777777777907"/>
+          <c:x val="0.86773547094188586"/>
+          <c:y val="0.37152777777777918"/>
           <c:w val="0.11422845691382746"/>
           <c:h val="0.25"/>
         </c:manualLayout>
@@ -974,7 +983,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000611" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000611" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000622" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000622" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1304,7 +1313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
@@ -2320,8 +2329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F163"/>
   <sheetViews>
-    <sheetView topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="B138" sqref="B138"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="F143" sqref="F143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4372,6 +4381,40 @@
         <v>6</v>
       </c>
     </row>
+    <row r="138" spans="2:6">
+      <c r="B138" s="1">
+        <v>40502</v>
+      </c>
+      <c r="C138" t="s">
+        <v>47</v>
+      </c>
+      <c r="D138" t="s">
+        <v>167</v>
+      </c>
+      <c r="E138" t="s">
+        <v>168</v>
+      </c>
+      <c r="F138">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="139" spans="2:6">
+      <c r="B139" s="1">
+        <v>40503</v>
+      </c>
+      <c r="C139" t="s">
+        <v>47</v>
+      </c>
+      <c r="D139" t="s">
+        <v>169</v>
+      </c>
+      <c r="E139" t="s">
+        <v>168</v>
+      </c>
+      <c r="F139">
+        <v>1.5</v>
+      </c>
+    </row>
     <row r="163" spans="2:6">
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
@@ -4381,7 +4424,7 @@
       </c>
       <c r="F163" s="3">
         <f>SUM(F135:F162)</f>
-        <v>11</v>
+        <v>19.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
S-01031 - Se modifica el script de inicializacion para mejorar los umbrales - Se corrige grafic para una mejor visualizacion de las metricas - Se sube la primer version de la presentacion final
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="171">
   <si>
     <t>Id</t>
   </si>
@@ -526,6 +526,9 @@
   </si>
   <si>
     <t>Mejoras en la visualizacion del salario del agente</t>
+  </si>
+  <si>
+    <t>Mejoras en el script de inicializacion y presentacion final</t>
   </si>
 </sst>
 </file>
@@ -917,11 +920,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="66076672"/>
-        <c:axId val="66078208"/>
+        <c:axId val="57688064"/>
+        <c:axId val="57689600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66076672"/>
+        <c:axId val="57688064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -945,14 +948,14 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66078208"/>
+        <c:crossAx val="57689600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66078208"/>
+        <c:axId val="57689600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -960,7 +963,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66076672"/>
+        <c:crossAx val="57688064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -971,8 +974,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86773547094188586"/>
-          <c:y val="0.37152777777777918"/>
+          <c:x val="0.86773547094188608"/>
+          <c:y val="0.37152777777777929"/>
           <c:w val="0.11422845691382746"/>
           <c:h val="0.25"/>
         </c:manualLayout>
@@ -983,7 +986,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000622" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000622" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000633" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000633" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2330,7 +2333,7 @@
   <dimension ref="B1:F163"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="F143" sqref="F143"/>
+      <selection activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4415,6 +4418,23 @@
         <v>1.5</v>
       </c>
     </row>
+    <row r="140" spans="2:6">
+      <c r="B140" s="1">
+        <v>40503</v>
+      </c>
+      <c r="C140" t="s">
+        <v>47</v>
+      </c>
+      <c r="D140" t="s">
+        <v>170</v>
+      </c>
+      <c r="E140" t="s">
+        <v>168</v>
+      </c>
+      <c r="F140">
+        <v>5</v>
+      </c>
+    </row>
     <row r="163" spans="2:6">
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
@@ -4424,7 +4444,7 @@
       </c>
       <c r="F163" s="3">
         <f>SUM(F135:F162)</f>
-        <v>19.5</v>
+        <v>24.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correccion en metricas totales y excel de metricas campaña 3
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="172">
   <si>
     <t>Id</t>
   </si>
@@ -529,6 +529,9 @@
   </si>
   <si>
     <t>Mejoras en el script de inicializacion y presentacion final</t>
+  </si>
+  <si>
+    <t>Correccion en metricas totales y excel de metricas campaña 3</t>
   </si>
 </sst>
 </file>
@@ -920,11 +923,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="57688064"/>
-        <c:axId val="57689600"/>
+        <c:axId val="59260928"/>
+        <c:axId val="59262464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57688064"/>
+        <c:axId val="59260928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -948,14 +951,14 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57689600"/>
+        <c:crossAx val="59262464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57689600"/>
+        <c:axId val="59262464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -963,7 +966,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57688064"/>
+        <c:crossAx val="59260928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -974,8 +977,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86773547094188608"/>
-          <c:y val="0.37152777777777929"/>
+          <c:x val="0.8677354709418863"/>
+          <c:y val="0.37152777777777946"/>
           <c:w val="0.11422845691382746"/>
           <c:h val="0.25"/>
         </c:manualLayout>
@@ -986,7 +989,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000633" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000633" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000644" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000644" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2332,8 +2335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="F141" sqref="F141"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="E141" sqref="E141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4435,6 +4438,20 @@
         <v>5</v>
       </c>
     </row>
+    <row r="141" spans="2:6">
+      <c r="B141" s="1">
+        <v>40504</v>
+      </c>
+      <c r="C141" t="s">
+        <v>47</v>
+      </c>
+      <c r="D141" t="s">
+        <v>171</v>
+      </c>
+      <c r="F141">
+        <v>6</v>
+      </c>
+    </row>
     <row r="163" spans="2:6">
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
@@ -4444,7 +4461,7 @@
       </c>
       <c r="F163" s="3">
         <f>SUM(F135:F162)</f>
-        <v>24.5</v>
+        <v>30.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se actualiza la métrica EV y primera version del reporte de avance del 25-11-2010 (falta actualizar FC)
</commit_message>
<xml_diff>
--- a/Documentacion/Minutas e informes/EarnedValue.xlsx
+++ b/Documentacion/Minutas e informes/EarnedValue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Earned Value" sheetId="1" r:id="rId1"/>
@@ -798,7 +798,7 @@
                   <c:v>293</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>333</c:v>
+                  <c:v>343</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -859,6 +859,9 @@
                 <c:pt idx="3">
                   <c:v>288</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>338</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -918,16 +921,19 @@
                 <c:pt idx="3">
                   <c:v>257</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>316</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="59260928"/>
-        <c:axId val="59262464"/>
+        <c:axId val="84425728"/>
+        <c:axId val="84439808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="59260928"/>
+        <c:axId val="84425728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -951,14 +957,14 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59262464"/>
+        <c:crossAx val="84439808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59262464"/>
+        <c:axId val="84439808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -966,7 +972,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59260928"/>
+        <c:crossAx val="84425728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -977,8 +983,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.8677354709418863"/>
-          <c:y val="0.37152777777777946"/>
+          <c:x val="0.86773547094188652"/>
+          <c:y val="0.37152777777777957"/>
           <c:w val="0.11422845691382746"/>
           <c:h val="0.25"/>
         </c:manualLayout>
@@ -989,7 +995,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000644" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000644" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000655" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000655" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2335,7 +2341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+    <sheetView topLeftCell="A130" workbookViewId="0">
       <selection activeCell="E141" sqref="E141"/>
     </sheetView>
   </sheetViews>
@@ -4482,8 +4488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B19:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4644,26 +4650,29 @@
         <v>64</v>
       </c>
       <c r="C24" s="11">
-        <f>C23+40</f>
-        <v>333</v>
-      </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
+        <v>343</v>
+      </c>
+      <c r="D24" s="11">
+        <v>338</v>
+      </c>
+      <c r="E24" s="11">
+        <v>316</v>
+      </c>
       <c r="F24" s="11">
         <f>D24-E24</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G24" s="11">
         <f>D24-C24</f>
-        <v>-333</v>
+        <v>-5</v>
       </c>
       <c r="H24" s="11">
         <f>D24/C24</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="11" t="e">
+        <v>0.98542274052478129</v>
+      </c>
+      <c r="I24" s="11">
         <f>D24/E24</f>
-        <v>#DIV/0!</v>
+        <v>1.0696202531645569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>